<commit_message>
Download EA form at details page
</commit_message>
<xml_diff>
--- a/assets/excel/ea_form.xlsx
+++ b/assets/excel/ea_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\faster-ea\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC594B08-0969-461C-81B9-3CEFA6601284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED66A47-61EE-45E6-B2DA-757DA6AC9BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,14 +139,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="114">
   <si>
     <t>DOMESTIC AND INTERNATIONAL EXPENSE AUTHORIZATION</t>
   </si>
   <si>
-    <t>EA No. EA21153</t>
-  </si>
-  <si>
     <t xml:space="preserve">Request Date:  </t>
   </si>
   <si>
@@ -156,21 +153,9 @@
     <t>A</t>
   </si>
   <si>
-    <t>Jessie Olivia Yunus</t>
-  </si>
-  <si>
     <t>Originating City</t>
   </si>
   <si>
-    <t>Jakarta</t>
-  </si>
-  <si>
-    <t>EPiC
-Generali Tower, 18th floor, Gran Rubina business Park, Rasuna Apicentrum
-Jl HR Rasuna Said Kav C22 Kuningan 
-Jakarta 12940 - Indonesia</t>
-  </si>
-  <si>
     <t>Departure Date</t>
   </si>
   <si>
@@ -180,9 +165,6 @@
     <t>Initiating BU:</t>
   </si>
   <si>
-    <t>EpiC</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -192,9 +174,6 @@
     <t>E</t>
   </si>
   <si>
-    <t>jyunus@fhi360.org</t>
-  </si>
-  <si>
     <t>Max budget amount for airfare</t>
   </si>
   <si>
@@ -204,15 +183,9 @@
     <t>F</t>
   </si>
   <si>
-    <t>Employee #114530</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t xml:space="preserve">Employee - </t>
   </si>
   <si>
@@ -237,9 +210,6 @@
     <t>City/Country:</t>
   </si>
   <si>
-    <t xml:space="preserve">Kota Tangerang </t>
-  </si>
-  <si>
     <t>Arr. Date:</t>
   </si>
   <si>
@@ -264,9 +234,6 @@
     <t>I</t>
   </si>
   <si>
-    <t>102533.034.001.001.001</t>
-  </si>
-  <si>
     <t>Item 1</t>
   </si>
   <si>
@@ -301,9 +268,6 @@
   </si>
   <si>
     <t>2nd Destination</t>
-  </si>
-  <si>
-    <t>Kota Tangerang Selatan</t>
   </si>
   <si>
     <t>Justification for each FCO/ID/project</t>
@@ -2724,8 +2688,8 @@
   </sheetPr>
   <dimension ref="A1:BC681"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="64" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:U21"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A73" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="64" workbookViewId="0">
+      <selection activeCell="W39" activeCellId="2" sqref="G39:M39 P39:S39 W39:AC39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -2815,9 +2779,7 @@
       <c r="AH2" s="213"/>
       <c r="AI2" s="213"/>
       <c r="AJ2" s="213"/>
-      <c r="AK2" s="205" t="s">
-        <v>1</v>
-      </c>
+      <c r="AK2" s="205"/>
       <c r="AL2" s="206"/>
       <c r="AM2" s="206"/>
       <c r="AN2" s="207"/>
@@ -2998,16 +2960,14 @@
       <c r="V6" s="12"/>
       <c r="W6" s="4"/>
       <c r="X6" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y6" s="13"/>
       <c r="Z6" s="13"/>
       <c r="AA6" s="84"/>
       <c r="AB6" s="84"/>
       <c r="AC6" s="84"/>
-      <c r="AD6" s="216">
-        <v>44508</v>
-      </c>
+      <c r="AD6" s="216"/>
       <c r="AE6" s="216"/>
       <c r="AF6" s="216"/>
       <c r="AG6" s="216"/>
@@ -3021,7 +2981,7 @@
       <c r="AO6" s="4"/>
       <c r="AP6" s="15"/>
       <c r="AQ6" s="115" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AR6" s="116"/>
       <c r="AS6" s="116"/>
@@ -3038,12 +2998,10 @@
     </row>
     <row r="7" spans="1:55" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="225" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="119" t="s">
-        <v>5</v>
-      </c>
+      <c r="C7" s="119"/>
       <c r="D7" s="120"/>
       <c r="E7" s="120"/>
       <c r="F7" s="120"/>
@@ -3102,16 +3060,14 @@
       <c r="U8" s="124"/>
       <c r="V8" s="12"/>
       <c r="X8" s="129" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Y8" s="129"/>
       <c r="Z8" s="129"/>
       <c r="AA8" s="129"/>
       <c r="AB8" s="129"/>
       <c r="AC8" s="129"/>
-      <c r="AD8" s="130" t="s">
-        <v>7</v>
-      </c>
+      <c r="AD8" s="130"/>
       <c r="AE8" s="130"/>
       <c r="AF8" s="130"/>
       <c r="AG8" s="130"/>
@@ -3123,7 +3079,7 @@
       <c r="AM8" s="130"/>
       <c r="AN8" s="14"/>
       <c r="AQ8" s="128" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AR8" s="128"/>
       <c r="AS8" s="128"/>
@@ -3195,9 +3151,7 @@
     <row r="10" spans="1:55" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="94"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="144" t="s">
-        <v>8</v>
-      </c>
+      <c r="C10" s="144"/>
       <c r="D10" s="145"/>
       <c r="E10" s="145"/>
       <c r="F10" s="145"/>
@@ -3218,16 +3172,14 @@
       <c r="U10" s="146"/>
       <c r="V10" s="16"/>
       <c r="X10" s="129" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Y10" s="129"/>
       <c r="Z10" s="129"/>
       <c r="AA10" s="129"/>
       <c r="AB10" s="129"/>
       <c r="AC10" s="129"/>
-      <c r="AD10" s="141">
-        <v>44514</v>
-      </c>
+      <c r="AD10" s="141"/>
       <c r="AE10" s="141"/>
       <c r="AF10" s="141"/>
       <c r="AG10" s="141"/>
@@ -3235,12 +3187,10 @@
       <c r="AI10" s="141"/>
       <c r="AJ10" s="141"/>
       <c r="AK10" s="134" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AL10" s="135"/>
-      <c r="AM10" s="137">
-        <v>44518</v>
-      </c>
+      <c r="AM10" s="137"/>
       <c r="AN10" s="14"/>
       <c r="AQ10" s="128"/>
       <c r="AR10" s="128"/>
@@ -3372,16 +3322,14 @@
       <c r="U13" s="149"/>
       <c r="V13" s="16"/>
       <c r="X13" s="143" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="Y13" s="143"/>
       <c r="Z13" s="143"/>
       <c r="AA13" s="143"/>
       <c r="AB13" s="143"/>
       <c r="AC13" s="143"/>
-      <c r="AG13" s="117" t="s">
-        <v>12</v>
-      </c>
+      <c r="AG13" s="117"/>
       <c r="AH13" s="117"/>
       <c r="AI13" s="118"/>
       <c r="AJ13" s="118"/>
@@ -3390,7 +3338,7 @@
       <c r="AM13" s="118"/>
       <c r="AN13" s="14"/>
       <c r="AQ13" s="94" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="AR13" s="94"/>
       <c r="AS13" s="94"/>
@@ -3471,7 +3419,7 @@
       <c r="V15" s="16"/>
       <c r="W15" s="21"/>
       <c r="X15" s="220" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="Y15" s="220"/>
       <c r="Z15" s="220"/>
@@ -3485,16 +3433,14 @@
       <c r="AH15" s="220"/>
       <c r="AI15" s="220"/>
       <c r="AJ15" s="220"/>
-      <c r="AK15" s="132" t="s">
-        <v>5</v>
-      </c>
+      <c r="AK15" s="132"/>
       <c r="AL15" s="132"/>
       <c r="AM15" s="132"/>
       <c r="AN15" s="133"/>
       <c r="AO15" s="23"/>
       <c r="AP15" s="23"/>
       <c r="AQ15" s="94" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AR15" s="94"/>
       <c r="AS15" s="94"/>
@@ -3512,9 +3458,7 @@
     <row r="16" spans="1:55" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="94"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="242" t="s">
-        <v>16</v>
-      </c>
+      <c r="C16" s="242"/>
       <c r="D16" s="243"/>
       <c r="E16" s="243"/>
       <c r="F16" s="243"/>
@@ -3536,7 +3480,7 @@
       <c r="V16" s="16"/>
       <c r="W16" s="24"/>
       <c r="X16" s="240" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="Y16" s="240"/>
       <c r="Z16" s="240"/>
@@ -3552,12 +3496,12 @@
       <c r="AJ16" s="240"/>
       <c r="AK16" s="240"/>
       <c r="AL16" s="238" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="AM16" s="238"/>
       <c r="AN16" s="239"/>
       <c r="AQ16" s="98" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:49" ht="5.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3567,9 +3511,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="230" t="s">
-        <v>20</v>
-      </c>
+      <c r="G17" s="230"/>
       <c r="H17" s="230"/>
       <c r="I17" s="230"/>
       <c r="J17" s="230"/>
@@ -3590,14 +3532,12 @@
     </row>
     <row r="18" spans="1:49" ht="5.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="226" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B18" s="5"/>
-      <c r="C18" s="162" t="s">
-        <v>22</v>
-      </c>
+      <c r="C18" s="162"/>
       <c r="D18" s="175" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E18" s="176"/>
       <c r="F18" s="176"/>
@@ -3621,7 +3561,7 @@
       <c r="X18" s="222"/>
       <c r="Y18" s="140"/>
       <c r="Z18" s="228" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="AA18" s="228"/>
       <c r="AB18" s="228"/>
@@ -3724,7 +3664,7 @@
       <c r="B21" s="5"/>
       <c r="C21" s="53"/>
       <c r="D21" s="175" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E21" s="176"/>
       <c r="F21" s="176"/>
@@ -3746,7 +3686,7 @@
       <c r="V21" s="32"/>
       <c r="W21" s="24"/>
       <c r="X21" s="176" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="Y21" s="176"/>
       <c r="Z21" s="176"/>
@@ -3813,12 +3753,12 @@
       <c r="B23" s="5"/>
       <c r="C23" s="53"/>
       <c r="D23" s="175" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E23" s="176"/>
       <c r="F23" s="176"/>
       <c r="G23" s="4" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
@@ -3902,7 +3842,7 @@
       <c r="A25" s="94"/>
       <c r="B25" s="5"/>
       <c r="C25" s="85" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D25" s="86"/>
       <c r="E25" s="86"/>
@@ -3937,18 +3877,16 @@
     </row>
     <row r="26" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="97" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="153" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D26" s="153"/>
       <c r="E26" s="153"/>
       <c r="F26" s="153"/>
-      <c r="G26" s="179" t="s">
-        <v>31</v>
-      </c>
+      <c r="G26" s="179"/>
       <c r="H26" s="118"/>
       <c r="I26" s="118"/>
       <c r="J26" s="118"/>
@@ -3956,22 +3894,18 @@
       <c r="L26" s="118"/>
       <c r="M26" s="118"/>
       <c r="O26" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="P26" s="177">
-        <v>44514</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="P26" s="177"/>
       <c r="Q26" s="212"/>
       <c r="R26" s="212"/>
       <c r="S26" s="212"/>
       <c r="T26" s="36"/>
       <c r="U26" s="154" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="V26" s="155"/>
-      <c r="W26" s="180">
-        <v>44518</v>
-      </c>
+      <c r="W26" s="180"/>
       <c r="X26" s="180"/>
       <c r="Y26" s="180"/>
       <c r="Z26" s="180"/>
@@ -3980,14 +3914,14 @@
       <c r="AC26" s="180"/>
       <c r="AG26" s="37"/>
       <c r="AH26" s="34" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="AN26" s="18"/>
       <c r="AW26" s="6"/>
     </row>
     <row r="27" spans="1:49" ht="5.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="227" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B27" s="5"/>
       <c r="AG27" s="37"/>
@@ -3998,7 +3932,7 @@
       <c r="A28" s="227"/>
       <c r="B28" s="5"/>
       <c r="C28" s="69" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D28" s="69"/>
       <c r="E28" s="69"/>
@@ -4010,7 +3944,7 @@
       <c r="K28" s="112"/>
       <c r="L28" s="112"/>
       <c r="M28" s="73" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="N28" s="113"/>
       <c r="O28" s="113"/>
@@ -4031,23 +3965,19 @@
       <c r="AD28" s="34"/>
       <c r="AG28" s="37"/>
       <c r="AJ28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL28" s="160">
-        <v>1200000</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="AL28" s="160"/>
       <c r="AM28" s="160"/>
       <c r="AN28" s="161"/>
       <c r="AW28" s="6"/>
     </row>
     <row r="29" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="96" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="C29" s="173" t="s">
-        <v>40</v>
-      </c>
+      <c r="C29" s="173"/>
       <c r="D29" s="173"/>
       <c r="E29" s="173"/>
       <c r="F29" s="173"/>
@@ -4077,7 +4007,7 @@
       <c r="AG29" s="37"/>
       <c r="AN29" s="18"/>
       <c r="AW29" s="38" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4113,24 +4043,22 @@
       <c r="AE30" s="36"/>
       <c r="AG30" s="37"/>
       <c r="AJ30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL30" s="160">
-        <v>520000</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="AL30" s="160"/>
       <c r="AM30" s="160"/>
       <c r="AN30" s="161"/>
       <c r="AW30" s="38" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:49" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="97" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="229" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D31" s="229"/>
       <c r="E31" s="229"/>
@@ -4163,7 +4091,7 @@
       <c r="AG31" s="37"/>
       <c r="AN31" s="18"/>
       <c r="AW31" s="38" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4200,16 +4128,16 @@
       <c r="AE32" s="20"/>
       <c r="AG32" s="37"/>
       <c r="AJ32" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="AL32" s="158">
         <f>AL28+AL30</f>
-        <v>1720000</v>
+        <v>0</v>
       </c>
       <c r="AM32" s="158"/>
       <c r="AN32" s="159"/>
       <c r="AW32" s="38" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4286,11 +4214,9 @@
       <c r="AE34" s="26"/>
       <c r="AG34" s="37"/>
       <c r="AJ34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL34" s="156">
-        <v>8</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="AL34" s="156"/>
       <c r="AM34" s="156"/>
       <c r="AN34" s="157"/>
       <c r="AW34" s="38"/>
@@ -4369,17 +4295,17 @@
       <c r="AE36" s="36"/>
       <c r="AG36" s="37"/>
       <c r="AJ36" s="34" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="AK36" s="34"/>
       <c r="AL36" s="158">
         <f>(AL30+AL28)*AL34</f>
-        <v>13760000</v>
+        <v>0</v>
       </c>
       <c r="AM36" s="158"/>
       <c r="AN36" s="159"/>
       <c r="AW36" s="38" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:49" ht="4.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4424,14 +4350,14 @@
       <c r="AM37" s="30"/>
       <c r="AN37" s="31"/>
       <c r="AW37" s="38" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:49" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="94"/>
       <c r="B38" s="5"/>
       <c r="C38" s="174" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D38" s="174"/>
       <c r="E38" s="174"/>
@@ -4466,18 +4392,16 @@
     </row>
     <row r="39" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="97" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="153" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D39" s="153"/>
       <c r="E39" s="153"/>
       <c r="F39" s="153"/>
-      <c r="G39" s="179" t="s">
-        <v>53</v>
-      </c>
+      <c r="G39" s="179"/>
       <c r="H39" s="118"/>
       <c r="I39" s="118"/>
       <c r="J39" s="118"/>
@@ -4485,22 +4409,18 @@
       <c r="L39" s="118"/>
       <c r="M39" s="118"/>
       <c r="O39" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="P39" s="177">
-        <v>44517</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="P39" s="177"/>
       <c r="Q39" s="178"/>
       <c r="R39" s="178"/>
       <c r="S39" s="178"/>
       <c r="T39" s="56"/>
       <c r="U39" s="154" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="V39" s="155"/>
-      <c r="W39" s="180">
-        <v>44517</v>
-      </c>
+      <c r="W39" s="180"/>
       <c r="X39" s="180"/>
       <c r="Y39" s="180"/>
       <c r="Z39" s="180"/>
@@ -4509,14 +4429,14 @@
       <c r="AC39" s="180"/>
       <c r="AG39" s="37"/>
       <c r="AH39" s="34" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="AN39" s="18"/>
       <c r="AW39" s="6"/>
     </row>
     <row r="40" spans="1:49" ht="5.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="227" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B40" s="5"/>
       <c r="AG40" s="37"/>
@@ -4527,7 +4447,7 @@
       <c r="A41" s="227"/>
       <c r="B41" s="5"/>
       <c r="C41" s="69" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D41" s="69"/>
       <c r="E41" s="69"/>
@@ -4539,7 +4459,7 @@
       <c r="K41" s="112"/>
       <c r="L41" s="112"/>
       <c r="M41" s="73" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="N41" s="113"/>
       <c r="O41" s="113"/>
@@ -4560,7 +4480,7 @@
       <c r="AD41" s="34"/>
       <c r="AG41" s="37"/>
       <c r="AJ41" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="AL41" s="160"/>
       <c r="AM41" s="160"/>
@@ -4569,7 +4489,7 @@
     </row>
     <row r="42" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="96" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="173"/>
@@ -4602,7 +4522,7 @@
       <c r="AG42" s="37"/>
       <c r="AN42" s="18"/>
       <c r="AW42" s="38" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4638,22 +4558,22 @@
       <c r="AE43" s="36"/>
       <c r="AG43" s="37"/>
       <c r="AJ43" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="AL43" s="160"/>
       <c r="AM43" s="160"/>
       <c r="AN43" s="161"/>
       <c r="AW43" s="38" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:49" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="97" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="75" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D44" s="76"/>
       <c r="E44" s="76"/>
@@ -4686,7 +4606,7 @@
       <c r="AG44" s="37"/>
       <c r="AN44" s="18"/>
       <c r="AW44" s="38" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4723,7 +4643,7 @@
       <c r="AE45" s="20"/>
       <c r="AG45" s="37"/>
       <c r="AJ45" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="AL45" s="158">
         <f>SUM(AL43+AL41)</f>
@@ -4732,7 +4652,7 @@
       <c r="AM45" s="158"/>
       <c r="AN45" s="159"/>
       <c r="AW45" s="38" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4809,7 +4729,7 @@
       <c r="AE47" s="26"/>
       <c r="AG47" s="37"/>
       <c r="AJ47" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="AL47" s="156"/>
       <c r="AM47" s="156"/>
@@ -4890,7 +4810,7 @@
       <c r="AE49" s="36"/>
       <c r="AG49" s="37"/>
       <c r="AJ49" s="34" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="AK49" s="34"/>
       <c r="AL49" s="158">
@@ -4900,7 +4820,7 @@
       <c r="AM49" s="158"/>
       <c r="AN49" s="159"/>
       <c r="AW49" s="38" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:49" ht="4.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4944,14 +4864,14 @@
       <c r="AM50" s="30"/>
       <c r="AN50" s="31"/>
       <c r="AW50" s="38" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:49" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="94"/>
       <c r="B51" s="7"/>
       <c r="C51" s="87" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D51" s="83"/>
       <c r="E51" s="83"/>
@@ -4986,11 +4906,11 @@
     </row>
     <row r="52" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="97" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="153" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D52" s="153"/>
       <c r="E52" s="153"/>
@@ -5003,7 +4923,7 @@
       <c r="L52" s="118"/>
       <c r="M52" s="118"/>
       <c r="O52" s="35" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="P52" s="177"/>
       <c r="Q52" s="178"/>
@@ -5011,7 +4931,7 @@
       <c r="S52" s="178"/>
       <c r="T52" s="56"/>
       <c r="U52" s="154" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="V52" s="155"/>
       <c r="W52" s="180"/>
@@ -5023,14 +4943,14 @@
       <c r="AC52" s="180"/>
       <c r="AG52" s="37"/>
       <c r="AH52" s="34" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="AN52" s="18"/>
       <c r="AW52" s="6"/>
     </row>
     <row r="53" spans="1:49" ht="5.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="227" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B53" s="5"/>
       <c r="AG53" s="37"/>
@@ -5041,7 +4961,7 @@
       <c r="A54" s="227"/>
       <c r="B54" s="5"/>
       <c r="C54" s="57" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D54" s="57"/>
       <c r="E54" s="57"/>
@@ -5049,7 +4969,7 @@
       <c r="G54" s="57"/>
       <c r="H54" s="17"/>
       <c r="M54" s="73" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="N54" s="113"/>
       <c r="O54" s="113"/>
@@ -5070,7 +4990,7 @@
       <c r="AD54" s="34"/>
       <c r="AG54" s="37"/>
       <c r="AJ54" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="AL54" s="160"/>
       <c r="AM54" s="160"/>
@@ -5079,7 +4999,7 @@
     </row>
     <row r="55" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="96" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="173"/>
@@ -5112,7 +5032,7 @@
       <c r="AG55" s="37"/>
       <c r="AN55" s="18"/>
       <c r="AW55" s="38" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5127,22 +5047,22 @@
       <c r="AE56" s="36"/>
       <c r="AG56" s="37"/>
       <c r="AJ56" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="AL56" s="160"/>
       <c r="AM56" s="160"/>
       <c r="AN56" s="161"/>
       <c r="AW56" s="38" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:49" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="97" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="75" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="D57" s="76"/>
       <c r="E57" s="76"/>
@@ -5175,7 +5095,7 @@
       <c r="AG57" s="37"/>
       <c r="AN57" s="18"/>
       <c r="AW57" s="38" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5212,7 +5132,7 @@
       <c r="AE58" s="20"/>
       <c r="AG58" s="37"/>
       <c r="AJ58" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="AL58" s="158">
         <f>SUM(AL56+AL54)</f>
@@ -5221,7 +5141,7 @@
       <c r="AM58" s="158"/>
       <c r="AN58" s="159"/>
       <c r="AW58" s="38" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5298,7 +5218,7 @@
       <c r="AE60" s="26"/>
       <c r="AG60" s="37"/>
       <c r="AJ60" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="AL60" s="156"/>
       <c r="AM60" s="156"/>
@@ -5379,7 +5299,7 @@
       <c r="AE62" s="36"/>
       <c r="AG62" s="37"/>
       <c r="AJ62" s="34" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="AK62" s="34"/>
       <c r="AL62" s="158">
@@ -5389,7 +5309,7 @@
       <c r="AM62" s="158"/>
       <c r="AN62" s="159"/>
       <c r="AW62" s="38" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:49" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5434,7 +5354,7 @@
       <c r="AM63" s="30"/>
       <c r="AN63" s="31"/>
       <c r="AW63" s="38" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:49" ht="9.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5447,11 +5367,11 @@
     </row>
     <row r="65" spans="1:48" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="94" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B65" s="5"/>
       <c r="C65" s="182" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D65" s="182"/>
       <c r="E65" s="182"/>
@@ -5463,7 +5383,7 @@
       <c r="K65" s="182"/>
       <c r="L65" s="36"/>
       <c r="T65" s="235" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="U65" s="236"/>
       <c r="V65" s="236"/>
@@ -5479,7 +5399,7 @@
       <c r="AF65" s="236"/>
       <c r="AG65" s="37"/>
       <c r="AH65" s="34" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="AI65" s="34"/>
       <c r="AJ65" s="34"/>
@@ -5502,30 +5422,30 @@
       <c r="A67" s="94"/>
       <c r="B67" s="5"/>
       <c r="U67" s="232" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="V67" s="232"/>
       <c r="W67" s="232"/>
       <c r="X67" s="140" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="Y67" s="140"/>
       <c r="Z67" s="140"/>
       <c r="AA67" s="140" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="AB67" s="140"/>
       <c r="AC67" s="140"/>
       <c r="AD67" s="24"/>
       <c r="AG67" s="37"/>
       <c r="AH67" s="143" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="AI67" s="181"/>
       <c r="AJ67" s="181"/>
       <c r="AK67" s="181"/>
       <c r="AL67" s="203" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="AM67" s="203"/>
       <c r="AN67" s="204"/>
@@ -5535,7 +5455,7 @@
       <c r="A68" s="94"/>
       <c r="B68" s="5"/>
       <c r="C68" s="112" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D68" s="112"/>
       <c r="E68" s="112"/>
@@ -5570,7 +5490,7 @@
       <c r="B69" s="5"/>
       <c r="C69" s="112"/>
       <c r="D69" s="202" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E69" s="202"/>
       <c r="F69" s="202"/>
@@ -5594,14 +5514,14 @@
       <c r="Y69" s="8"/>
       <c r="AG69" s="37"/>
       <c r="AH69" s="143" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="AI69" s="181"/>
       <c r="AJ69" s="181"/>
       <c r="AK69" s="181"/>
       <c r="AL69" s="158">
         <f>+AL62+AL49+AL36</f>
-        <v>13760000</v>
+        <v>0</v>
       </c>
       <c r="AM69" s="158"/>
       <c r="AN69" s="159"/>
@@ -5643,7 +5563,7 @@
       <c r="A71" s="94"/>
       <c r="B71" s="5"/>
       <c r="C71" s="196" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D71" s="196"/>
       <c r="E71" s="196"/>
@@ -5670,7 +5590,7 @@
       <c r="AD71" s="36"/>
       <c r="AG71" s="37"/>
       <c r="AH71" s="143" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="AI71" s="143"/>
       <c r="AJ71" s="143"/>
@@ -5686,7 +5606,7 @@
       <c r="A72" s="94"/>
       <c r="B72" s="5"/>
       <c r="C72" s="196" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D72" s="196"/>
       <c r="E72" s="196"/>
@@ -5722,7 +5642,7 @@
       <c r="A73" s="94"/>
       <c r="B73" s="5"/>
       <c r="C73" s="196" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D73" s="196"/>
       <c r="E73" s="196"/>
@@ -5749,7 +5669,7 @@
       <c r="AC73" s="155"/>
       <c r="AG73" s="37"/>
       <c r="AH73" s="143" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="AI73" s="143"/>
       <c r="AJ73" s="143"/>
@@ -5763,7 +5683,7 @@
       <c r="A74" s="94"/>
       <c r="B74" s="5"/>
       <c r="C74" s="80" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D74" s="62"/>
       <c r="E74" s="62"/>
@@ -5798,7 +5718,7 @@
       <c r="A75" s="94"/>
       <c r="B75" s="5"/>
       <c r="C75" s="200" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D75" s="201"/>
       <c r="E75" s="201"/>
@@ -5861,7 +5781,7 @@
       <c r="AG76" s="37"/>
       <c r="AL76" s="79">
         <f>SUM(AL68:AN73)</f>
-        <v>14760000</v>
+        <v>1000000</v>
       </c>
       <c r="AM76" s="79"/>
       <c r="AN76" s="59"/>
@@ -5871,7 +5791,7 @@
       <c r="A77" s="94"/>
       <c r="B77" s="5"/>
       <c r="C77" s="190" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D77" s="191"/>
       <c r="E77" s="191"/>
@@ -5901,14 +5821,14 @@
       <c r="AC77" s="192"/>
       <c r="AG77" s="37"/>
       <c r="AH77" s="143" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="AI77" s="143"/>
       <c r="AJ77" s="143"/>
       <c r="AK77" s="143"/>
       <c r="AL77" s="158">
         <f>SUM(AL69:AN73)</f>
-        <v>14760000</v>
+        <v>1000000</v>
       </c>
       <c r="AM77" s="158"/>
       <c r="AN77" s="159"/>
@@ -5982,7 +5902,7 @@
       <c r="AC79" s="192"/>
       <c r="AG79" s="37"/>
       <c r="AH79" s="143" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="AI79" s="181"/>
       <c r="AJ79" s="181"/>
@@ -6062,14 +5982,14 @@
       <c r="AC81" s="192"/>
       <c r="AG81" s="37"/>
       <c r="AH81" s="143" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="AI81" s="181"/>
       <c r="AJ81" s="181"/>
       <c r="AK81" s="181"/>
       <c r="AL81" s="198">
         <f>ROUND(SUM(AL79*AL77),0)</f>
-        <v>11808000</v>
+        <v>800000</v>
       </c>
       <c r="AM81" s="198"/>
       <c r="AN81" s="199"/>
@@ -6178,7 +6098,7 @@
     </row>
     <row r="86" spans="1:52" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="94" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B86" s="5"/>
       <c r="C86" s="241"/>
@@ -6194,7 +6114,7 @@
       <c r="M86" s="241"/>
       <c r="N86" s="241"/>
       <c r="O86" s="249" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="P86" s="250"/>
       <c r="Q86" s="250"/>
@@ -6227,7 +6147,7 @@
       <c r="A87" s="94"/>
       <c r="B87" s="5"/>
       <c r="C87" s="245" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D87" s="245"/>
       <c r="E87" s="245"/>
@@ -6357,7 +6277,7 @@
     </row>
     <row r="90" spans="1:52" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="94" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B90" s="5"/>
       <c r="C90" s="248"/>
@@ -6403,7 +6323,7 @@
       <c r="A91" s="94"/>
       <c r="B91" s="5"/>
       <c r="C91" s="251" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D91" s="251"/>
       <c r="E91" s="251"/>
@@ -6418,7 +6338,7 @@
       <c r="N91" s="251"/>
       <c r="O91" s="44"/>
       <c r="P91" s="108" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="Q91" s="108"/>
       <c r="R91" s="108"/>
@@ -6431,7 +6351,7 @@
       <c r="Y91" s="108"/>
       <c r="Z91" s="44"/>
       <c r="AC91" s="154" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="AD91" s="154"/>
       <c r="AE91" s="154"/>
@@ -6463,7 +6383,7 @@
       <c r="M92" s="44"/>
       <c r="N92" s="44"/>
       <c r="P92" s="103" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="Q92" s="103"/>
       <c r="R92" s="103"/>
@@ -6533,7 +6453,7 @@
       <c r="A94" s="94"/>
       <c r="B94" s="5"/>
       <c r="F94" s="237" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G94" s="237"/>
       <c r="H94" s="237"/>
@@ -7402,15 +7322,12 @@
       <formula2>8</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C16" r:id="rId1" xr:uid="{71552FA0-4D5E-4C6C-9B27-4E8BEC94D460}"/>
-  </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.18" right="0.18" top="0.17" bottom="0.46" header="0" footer="0"/>
-  <pageSetup scale="67" orientation="portrait" r:id="rId2"/>
+  <pageSetup scale="67" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -7430,7 +7347,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="255" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B1" s="256"/>
     </row>
@@ -7440,13 +7357,13 @@
     </row>
     <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="257" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B3" s="257"/>
     </row>
     <row r="4" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="257" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B4" s="257"/>
     </row>
@@ -7456,13 +7373,13 @@
     </row>
     <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="258" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B6" s="258"/>
     </row>
     <row r="7" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="259" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B7" s="259"/>
     </row>
@@ -7472,114 +7389,114 @@
     </row>
     <row r="9" spans="1:2" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A9" s="89" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B9" s="90" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="31" x14ac:dyDescent="0.25">
       <c r="A10" s="91" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B10" s="90" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="31" x14ac:dyDescent="0.25">
       <c r="A11" s="91" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B11" s="90" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="89" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B12" s="92" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="89" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B13" s="90" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="89" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B14" s="90" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="31" x14ac:dyDescent="0.25">
       <c r="A15" s="91" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B15" s="90" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="91" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B16" s="90" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="61" x14ac:dyDescent="0.25">
       <c r="A17" s="91" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B17" s="90" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="91" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B18" s="93" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="62" x14ac:dyDescent="0.25">
       <c r="A19" s="89" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B19" s="90" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="91" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B20" s="90" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30.5" x14ac:dyDescent="0.25">
       <c r="A21" s="91" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B21" s="90" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="100" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B22" s="101" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.5" x14ac:dyDescent="0.25">
@@ -7588,10 +7505,10 @@
     </row>
     <row r="24" spans="1:2" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A24" s="91" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B24" s="90" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.5" x14ac:dyDescent="0.25">
@@ -7600,7 +7517,7 @@
     </row>
     <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="99" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7609,7 +7526,7 @@
     </row>
     <row r="28" spans="1:2" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="253" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B28" s="254"/>
     </row>

</xml_diff>

<commit_message>
Attach file excel for all level on application
</commit_message>
<xml_diff>
--- a/assets/excel/ea_form.xlsx
+++ b/assets/excel/ea_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\faster-ea\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFFC732-E35B-48C3-B562-797F6885BD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670CDD4D-35A8-4BFC-BCD9-2C8B86347EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1254,7 +1254,7 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="260">
+  <cellXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1645,18 +1645,6 @@
       <alignment horizontal="right" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -2082,6 +2070,14 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2594,8 +2590,8 @@
   </sheetPr>
   <dimension ref="A1:BC681"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A79" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="64" workbookViewId="0">
-      <selection activeCell="W39" activeCellId="2" sqref="G39:M39 P39:S39 W39:AC39"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A76" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="64" workbookViewId="0">
+      <selection activeCell="I89" sqref="I89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -2656,39 +2652,39 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="172" t="s">
+      <c r="J2" s="169" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="172"/>
-      <c r="L2" s="172"/>
-      <c r="M2" s="172"/>
-      <c r="N2" s="172"/>
-      <c r="O2" s="172"/>
-      <c r="P2" s="172"/>
-      <c r="Q2" s="172"/>
-      <c r="R2" s="172"/>
-      <c r="S2" s="172"/>
-      <c r="T2" s="172"/>
-      <c r="U2" s="172"/>
-      <c r="V2" s="172"/>
-      <c r="W2" s="172"/>
-      <c r="X2" s="172"/>
-      <c r="Y2" s="172"/>
-      <c r="Z2" s="172"/>
-      <c r="AA2" s="172"/>
-      <c r="AB2" s="172"/>
-      <c r="AC2" s="172"/>
-      <c r="AD2" s="172"/>
-      <c r="AE2" s="172"/>
-      <c r="AF2" s="172"/>
-      <c r="AG2" s="172"/>
-      <c r="AH2" s="172"/>
-      <c r="AI2" s="172"/>
-      <c r="AJ2" s="172"/>
-      <c r="AK2" s="164"/>
-      <c r="AL2" s="165"/>
-      <c r="AM2" s="165"/>
-      <c r="AN2" s="166"/>
+      <c r="K2" s="169"/>
+      <c r="L2" s="169"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
+      <c r="Q2" s="169"/>
+      <c r="R2" s="169"/>
+      <c r="S2" s="169"/>
+      <c r="T2" s="169"/>
+      <c r="U2" s="169"/>
+      <c r="V2" s="169"/>
+      <c r="W2" s="169"/>
+      <c r="X2" s="169"/>
+      <c r="Y2" s="169"/>
+      <c r="Z2" s="169"/>
+      <c r="AA2" s="169"/>
+      <c r="AB2" s="169"/>
+      <c r="AC2" s="169"/>
+      <c r="AD2" s="169"/>
+      <c r="AE2" s="169"/>
+      <c r="AF2" s="169"/>
+      <c r="AG2" s="169"/>
+      <c r="AH2" s="169"/>
+      <c r="AI2" s="169"/>
+      <c r="AJ2" s="169"/>
+      <c r="AK2" s="161"/>
+      <c r="AL2" s="162"/>
+      <c r="AM2" s="162"/>
+      <c r="AN2" s="163"/>
       <c r="AO2" s="4"/>
       <c r="AP2" s="4"/>
       <c r="AQ2" s="4"/>
@@ -2697,37 +2693,37 @@
     <row r="3" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="94"/>
       <c r="B3" s="5"/>
-      <c r="J3" s="173"/>
-      <c r="K3" s="173"/>
-      <c r="L3" s="173"/>
-      <c r="M3" s="173"/>
-      <c r="N3" s="173"/>
-      <c r="O3" s="173"/>
-      <c r="P3" s="173"/>
-      <c r="Q3" s="173"/>
-      <c r="R3" s="173"/>
-      <c r="S3" s="173"/>
-      <c r="T3" s="173"/>
-      <c r="U3" s="173"/>
-      <c r="V3" s="173"/>
-      <c r="W3" s="173"/>
-      <c r="X3" s="173"/>
-      <c r="Y3" s="173"/>
-      <c r="Z3" s="173"/>
-      <c r="AA3" s="173"/>
-      <c r="AB3" s="173"/>
-      <c r="AC3" s="173"/>
-      <c r="AD3" s="173"/>
-      <c r="AE3" s="173"/>
-      <c r="AF3" s="173"/>
-      <c r="AG3" s="173"/>
-      <c r="AH3" s="173"/>
-      <c r="AI3" s="173"/>
-      <c r="AJ3" s="173"/>
-      <c r="AK3" s="167"/>
-      <c r="AL3" s="167"/>
-      <c r="AM3" s="167"/>
-      <c r="AN3" s="168"/>
+      <c r="J3" s="170"/>
+      <c r="K3" s="170"/>
+      <c r="L3" s="170"/>
+      <c r="M3" s="170"/>
+      <c r="N3" s="170"/>
+      <c r="O3" s="170"/>
+      <c r="P3" s="170"/>
+      <c r="Q3" s="170"/>
+      <c r="R3" s="170"/>
+      <c r="S3" s="170"/>
+      <c r="T3" s="170"/>
+      <c r="U3" s="170"/>
+      <c r="V3" s="170"/>
+      <c r="W3" s="170"/>
+      <c r="X3" s="170"/>
+      <c r="Y3" s="170"/>
+      <c r="Z3" s="170"/>
+      <c r="AA3" s="170"/>
+      <c r="AB3" s="170"/>
+      <c r="AC3" s="170"/>
+      <c r="AD3" s="170"/>
+      <c r="AE3" s="170"/>
+      <c r="AF3" s="170"/>
+      <c r="AG3" s="170"/>
+      <c r="AH3" s="170"/>
+      <c r="AI3" s="170"/>
+      <c r="AJ3" s="170"/>
+      <c r="AK3" s="164"/>
+      <c r="AL3" s="164"/>
+      <c r="AM3" s="164"/>
+      <c r="AN3" s="165"/>
       <c r="AO3" s="4"/>
       <c r="AP3" s="4"/>
       <c r="AQ3" s="4"/>
@@ -2737,37 +2733,37 @@
     <row r="4" spans="1:55" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="94"/>
       <c r="B4" s="5"/>
-      <c r="J4" s="174"/>
-      <c r="K4" s="174"/>
-      <c r="L4" s="174"/>
-      <c r="M4" s="174"/>
-      <c r="N4" s="174"/>
-      <c r="O4" s="174"/>
-      <c r="P4" s="174"/>
-      <c r="Q4" s="174"/>
-      <c r="R4" s="174"/>
-      <c r="S4" s="174"/>
-      <c r="T4" s="174"/>
-      <c r="U4" s="174"/>
-      <c r="V4" s="174"/>
-      <c r="W4" s="174"/>
-      <c r="X4" s="174"/>
-      <c r="Y4" s="174"/>
-      <c r="Z4" s="174"/>
-      <c r="AA4" s="174"/>
-      <c r="AB4" s="174"/>
-      <c r="AC4" s="174"/>
-      <c r="AD4" s="174"/>
-      <c r="AE4" s="174"/>
-      <c r="AF4" s="174"/>
-      <c r="AG4" s="174"/>
-      <c r="AH4" s="174"/>
-      <c r="AI4" s="174"/>
-      <c r="AJ4" s="174"/>
-      <c r="AK4" s="169"/>
-      <c r="AL4" s="169"/>
-      <c r="AM4" s="169"/>
-      <c r="AN4" s="170"/>
+      <c r="J4" s="171"/>
+      <c r="K4" s="171"/>
+      <c r="L4" s="171"/>
+      <c r="M4" s="171"/>
+      <c r="N4" s="171"/>
+      <c r="O4" s="171"/>
+      <c r="P4" s="171"/>
+      <c r="Q4" s="171"/>
+      <c r="R4" s="171"/>
+      <c r="S4" s="171"/>
+      <c r="T4" s="171"/>
+      <c r="U4" s="171"/>
+      <c r="V4" s="171"/>
+      <c r="W4" s="171"/>
+      <c r="X4" s="171"/>
+      <c r="Y4" s="171"/>
+      <c r="Z4" s="171"/>
+      <c r="AA4" s="171"/>
+      <c r="AB4" s="171"/>
+      <c r="AC4" s="171"/>
+      <c r="AD4" s="171"/>
+      <c r="AE4" s="171"/>
+      <c r="AF4" s="171"/>
+      <c r="AG4" s="171"/>
+      <c r="AH4" s="171"/>
+      <c r="AI4" s="171"/>
+      <c r="AJ4" s="171"/>
+      <c r="AK4" s="166"/>
+      <c r="AL4" s="166"/>
+      <c r="AM4" s="166"/>
+      <c r="AN4" s="167"/>
       <c r="AO4" s="4"/>
       <c r="AP4" s="4"/>
       <c r="AQ4" s="95"/>
@@ -2873,24 +2869,24 @@
       <c r="AA6" s="84"/>
       <c r="AB6" s="84"/>
       <c r="AC6" s="84"/>
-      <c r="AD6" s="175"/>
-      <c r="AE6" s="175"/>
-      <c r="AF6" s="175"/>
-      <c r="AG6" s="175"/>
-      <c r="AH6" s="175"/>
-      <c r="AI6" s="175"/>
-      <c r="AJ6" s="175"/>
-      <c r="AK6" s="175"/>
-      <c r="AL6" s="175"/>
-      <c r="AM6" s="175"/>
+      <c r="AD6" s="172"/>
+      <c r="AE6" s="172"/>
+      <c r="AF6" s="172"/>
+      <c r="AG6" s="172"/>
+      <c r="AH6" s="172"/>
+      <c r="AI6" s="172"/>
+      <c r="AJ6" s="172"/>
+      <c r="AK6" s="172"/>
+      <c r="AL6" s="172"/>
+      <c r="AM6" s="172"/>
       <c r="AN6" s="14"/>
       <c r="AO6" s="4"/>
       <c r="AP6" s="15"/>
-      <c r="AQ6" s="230" t="s">
+      <c r="AQ6" s="227" t="s">
         <v>2</v>
       </c>
-      <c r="AR6" s="231"/>
-      <c r="AS6" s="231"/>
+      <c r="AR6" s="228"/>
+      <c r="AS6" s="228"/>
       <c r="AT6" s="94"/>
       <c r="AU6" s="94"/>
       <c r="AV6" s="94"/>
@@ -2903,29 +2899,29 @@
       <c r="BC6" s="94"/>
     </row>
     <row r="7" spans="1:55" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="146" t="s">
+      <c r="A7" s="143" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="233"/>
-      <c r="D7" s="234"/>
-      <c r="E7" s="234"/>
-      <c r="F7" s="234"/>
-      <c r="G7" s="234"/>
-      <c r="H7" s="234"/>
-      <c r="I7" s="234"/>
-      <c r="J7" s="234"/>
-      <c r="K7" s="234"/>
-      <c r="L7" s="234"/>
-      <c r="M7" s="234"/>
-      <c r="N7" s="234"/>
-      <c r="O7" s="234"/>
-      <c r="P7" s="234"/>
-      <c r="Q7" s="234"/>
-      <c r="R7" s="234"/>
-      <c r="S7" s="234"/>
-      <c r="T7" s="234"/>
-      <c r="U7" s="235"/>
+      <c r="C7" s="230"/>
+      <c r="D7" s="231"/>
+      <c r="E7" s="231"/>
+      <c r="F7" s="231"/>
+      <c r="G7" s="231"/>
+      <c r="H7" s="231"/>
+      <c r="I7" s="231"/>
+      <c r="J7" s="231"/>
+      <c r="K7" s="231"/>
+      <c r="L7" s="231"/>
+      <c r="M7" s="231"/>
+      <c r="N7" s="231"/>
+      <c r="O7" s="231"/>
+      <c r="P7" s="231"/>
+      <c r="Q7" s="231"/>
+      <c r="R7" s="231"/>
+      <c r="S7" s="231"/>
+      <c r="T7" s="231"/>
+      <c r="U7" s="232"/>
       <c r="V7" s="12"/>
       <c r="AN7" s="14"/>
       <c r="AQ7" s="94"/>
@@ -2943,214 +2939,214 @@
       <c r="BC7" s="94"/>
     </row>
     <row r="8" spans="1:55" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="146"/>
+      <c r="A8" s="143"/>
       <c r="B8" s="5"/>
-      <c r="C8" s="236"/>
-      <c r="D8" s="237"/>
-      <c r="E8" s="237"/>
-      <c r="F8" s="237"/>
-      <c r="G8" s="237"/>
-      <c r="H8" s="237"/>
-      <c r="I8" s="237"/>
-      <c r="J8" s="237"/>
-      <c r="K8" s="237"/>
-      <c r="L8" s="237"/>
-      <c r="M8" s="237"/>
-      <c r="N8" s="237"/>
-      <c r="O8" s="237"/>
-      <c r="P8" s="237"/>
-      <c r="Q8" s="237"/>
-      <c r="R8" s="237"/>
-      <c r="S8" s="237"/>
-      <c r="T8" s="237"/>
-      <c r="U8" s="238"/>
+      <c r="C8" s="233"/>
+      <c r="D8" s="234"/>
+      <c r="E8" s="234"/>
+      <c r="F8" s="234"/>
+      <c r="G8" s="234"/>
+      <c r="H8" s="234"/>
+      <c r="I8" s="234"/>
+      <c r="J8" s="234"/>
+      <c r="K8" s="234"/>
+      <c r="L8" s="234"/>
+      <c r="M8" s="234"/>
+      <c r="N8" s="234"/>
+      <c r="O8" s="234"/>
+      <c r="P8" s="234"/>
+      <c r="Q8" s="234"/>
+      <c r="R8" s="234"/>
+      <c r="S8" s="234"/>
+      <c r="T8" s="234"/>
+      <c r="U8" s="235"/>
       <c r="V8" s="12"/>
-      <c r="X8" s="243" t="s">
+      <c r="X8" s="240" t="s">
         <v>4</v>
       </c>
-      <c r="Y8" s="243"/>
-      <c r="Z8" s="243"/>
-      <c r="AA8" s="243"/>
-      <c r="AB8" s="243"/>
-      <c r="AC8" s="243"/>
-      <c r="AD8" s="244"/>
-      <c r="AE8" s="244"/>
-      <c r="AF8" s="244"/>
-      <c r="AG8" s="244"/>
-      <c r="AH8" s="244"/>
-      <c r="AI8" s="244"/>
-      <c r="AJ8" s="244"/>
-      <c r="AK8" s="244"/>
-      <c r="AL8" s="244"/>
-      <c r="AM8" s="244"/>
+      <c r="Y8" s="240"/>
+      <c r="Z8" s="240"/>
+      <c r="AA8" s="240"/>
+      <c r="AB8" s="240"/>
+      <c r="AC8" s="240"/>
+      <c r="AD8" s="241"/>
+      <c r="AE8" s="241"/>
+      <c r="AF8" s="241"/>
+      <c r="AG8" s="241"/>
+      <c r="AH8" s="241"/>
+      <c r="AI8" s="241"/>
+      <c r="AJ8" s="241"/>
+      <c r="AK8" s="241"/>
+      <c r="AL8" s="241"/>
+      <c r="AM8" s="241"/>
       <c r="AN8" s="14"/>
-      <c r="AQ8" s="242" t="s">
+      <c r="AQ8" s="239" t="s">
         <v>2</v>
       </c>
-      <c r="AR8" s="242"/>
-      <c r="AS8" s="242"/>
-      <c r="AT8" s="242"/>
-      <c r="AU8" s="242"/>
-      <c r="AV8" s="242"/>
-      <c r="AW8" s="242"/>
-      <c r="AX8" s="242"/>
-      <c r="AY8" s="242"/>
-      <c r="AZ8" s="242"/>
-      <c r="BA8" s="242"/>
-      <c r="BB8" s="242"/>
-      <c r="BC8" s="242"/>
+      <c r="AR8" s="239"/>
+      <c r="AS8" s="239"/>
+      <c r="AT8" s="239"/>
+      <c r="AU8" s="239"/>
+      <c r="AV8" s="239"/>
+      <c r="AW8" s="239"/>
+      <c r="AX8" s="239"/>
+      <c r="AY8" s="239"/>
+      <c r="AZ8" s="239"/>
+      <c r="BA8" s="239"/>
+      <c r="BB8" s="239"/>
+      <c r="BC8" s="239"/>
     </row>
     <row r="9" spans="1:55" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="94"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="239"/>
-      <c r="D9" s="240"/>
-      <c r="E9" s="240"/>
-      <c r="F9" s="240"/>
-      <c r="G9" s="240"/>
-      <c r="H9" s="240"/>
-      <c r="I9" s="240"/>
-      <c r="J9" s="240"/>
-      <c r="K9" s="240"/>
-      <c r="L9" s="240"/>
-      <c r="M9" s="240"/>
-      <c r="N9" s="240"/>
-      <c r="O9" s="240"/>
-      <c r="P9" s="240"/>
-      <c r="Q9" s="240"/>
-      <c r="R9" s="240"/>
-      <c r="S9" s="240"/>
-      <c r="T9" s="240"/>
-      <c r="U9" s="241"/>
+      <c r="C9" s="236"/>
+      <c r="D9" s="237"/>
+      <c r="E9" s="237"/>
+      <c r="F9" s="237"/>
+      <c r="G9" s="237"/>
+      <c r="H9" s="237"/>
+      <c r="I9" s="237"/>
+      <c r="J9" s="237"/>
+      <c r="K9" s="237"/>
+      <c r="L9" s="237"/>
+      <c r="M9" s="237"/>
+      <c r="N9" s="237"/>
+      <c r="O9" s="237"/>
+      <c r="P9" s="237"/>
+      <c r="Q9" s="237"/>
+      <c r="R9" s="237"/>
+      <c r="S9" s="237"/>
+      <c r="T9" s="237"/>
+      <c r="U9" s="238"/>
       <c r="V9" s="12"/>
-      <c r="X9" s="243"/>
-      <c r="Y9" s="243"/>
-      <c r="Z9" s="243"/>
-      <c r="AA9" s="243"/>
-      <c r="AB9" s="243"/>
-      <c r="AC9" s="243"/>
-      <c r="AD9" s="245"/>
-      <c r="AE9" s="245"/>
-      <c r="AF9" s="245"/>
-      <c r="AG9" s="245"/>
-      <c r="AH9" s="245"/>
-      <c r="AI9" s="245"/>
-      <c r="AJ9" s="245"/>
-      <c r="AK9" s="245"/>
-      <c r="AL9" s="245"/>
-      <c r="AM9" s="245"/>
+      <c r="X9" s="240"/>
+      <c r="Y9" s="240"/>
+      <c r="Z9" s="240"/>
+      <c r="AA9" s="240"/>
+      <c r="AB9" s="240"/>
+      <c r="AC9" s="240"/>
+      <c r="AD9" s="242"/>
+      <c r="AE9" s="242"/>
+      <c r="AF9" s="242"/>
+      <c r="AG9" s="242"/>
+      <c r="AH9" s="242"/>
+      <c r="AI9" s="242"/>
+      <c r="AJ9" s="242"/>
+      <c r="AK9" s="242"/>
+      <c r="AL9" s="242"/>
+      <c r="AM9" s="242"/>
       <c r="AN9" s="14"/>
-      <c r="AQ9" s="242"/>
-      <c r="AR9" s="242"/>
-      <c r="AS9" s="242"/>
-      <c r="AT9" s="242"/>
-      <c r="AU9" s="242"/>
-      <c r="AV9" s="242"/>
-      <c r="AW9" s="242"/>
-      <c r="AX9" s="242"/>
-      <c r="AY9" s="242"/>
-      <c r="AZ9" s="242"/>
-      <c r="BA9" s="242"/>
-      <c r="BB9" s="242"/>
-      <c r="BC9" s="242"/>
+      <c r="AQ9" s="239"/>
+      <c r="AR9" s="239"/>
+      <c r="AS9" s="239"/>
+      <c r="AT9" s="239"/>
+      <c r="AU9" s="239"/>
+      <c r="AV9" s="239"/>
+      <c r="AW9" s="239"/>
+      <c r="AX9" s="239"/>
+      <c r="AY9" s="239"/>
+      <c r="AZ9" s="239"/>
+      <c r="BA9" s="239"/>
+      <c r="BB9" s="239"/>
+      <c r="BC9" s="239"/>
     </row>
     <row r="10" spans="1:55" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="94"/>
       <c r="B10" s="5"/>
-      <c r="C10" s="218"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="219"/>
-      <c r="H10" s="219"/>
-      <c r="I10" s="219"/>
-      <c r="J10" s="219"/>
-      <c r="K10" s="219"/>
-      <c r="L10" s="219"/>
-      <c r="M10" s="219"/>
-      <c r="N10" s="219"/>
-      <c r="O10" s="219"/>
-      <c r="P10" s="219"/>
-      <c r="Q10" s="219"/>
-      <c r="R10" s="219"/>
-      <c r="S10" s="219"/>
-      <c r="T10" s="219"/>
-      <c r="U10" s="220"/>
+      <c r="C10" s="215"/>
+      <c r="D10" s="216"/>
+      <c r="E10" s="216"/>
+      <c r="F10" s="216"/>
+      <c r="G10" s="216"/>
+      <c r="H10" s="216"/>
+      <c r="I10" s="216"/>
+      <c r="J10" s="216"/>
+      <c r="K10" s="216"/>
+      <c r="L10" s="216"/>
+      <c r="M10" s="216"/>
+      <c r="N10" s="216"/>
+      <c r="O10" s="216"/>
+      <c r="P10" s="216"/>
+      <c r="Q10" s="216"/>
+      <c r="R10" s="216"/>
+      <c r="S10" s="216"/>
+      <c r="T10" s="216"/>
+      <c r="U10" s="217"/>
       <c r="V10" s="16"/>
-      <c r="X10" s="243" t="s">
+      <c r="X10" s="240" t="s">
         <v>5</v>
       </c>
-      <c r="Y10" s="243"/>
-      <c r="Z10" s="243"/>
-      <c r="AA10" s="243"/>
-      <c r="AB10" s="243"/>
-      <c r="AC10" s="243"/>
-      <c r="AD10" s="216"/>
-      <c r="AE10" s="216"/>
-      <c r="AF10" s="216"/>
-      <c r="AG10" s="216"/>
-      <c r="AH10" s="216"/>
-      <c r="AI10" s="216"/>
-      <c r="AJ10" s="216"/>
-      <c r="AK10" s="248" t="s">
+      <c r="Y10" s="240"/>
+      <c r="Z10" s="240"/>
+      <c r="AA10" s="240"/>
+      <c r="AB10" s="240"/>
+      <c r="AC10" s="240"/>
+      <c r="AD10" s="213"/>
+      <c r="AE10" s="213"/>
+      <c r="AF10" s="213"/>
+      <c r="AG10" s="213"/>
+      <c r="AH10" s="213"/>
+      <c r="AI10" s="213"/>
+      <c r="AJ10" s="213"/>
+      <c r="AK10" s="245" t="s">
         <v>6</v>
       </c>
-      <c r="AL10" s="249"/>
-      <c r="AM10" s="251"/>
+      <c r="AL10" s="246"/>
+      <c r="AM10" s="248"/>
       <c r="AN10" s="14"/>
-      <c r="AQ10" s="242"/>
-      <c r="AR10" s="242"/>
-      <c r="AS10" s="242"/>
-      <c r="AT10" s="242"/>
-      <c r="AU10" s="242"/>
-      <c r="AV10" s="242"/>
-      <c r="AW10" s="242"/>
-      <c r="AX10" s="242"/>
-      <c r="AY10" s="242"/>
-      <c r="AZ10" s="242"/>
-      <c r="BA10" s="242"/>
-      <c r="BB10" s="242"/>
-      <c r="BC10" s="242"/>
+      <c r="AQ10" s="239"/>
+      <c r="AR10" s="239"/>
+      <c r="AS10" s="239"/>
+      <c r="AT10" s="239"/>
+      <c r="AU10" s="239"/>
+      <c r="AV10" s="239"/>
+      <c r="AW10" s="239"/>
+      <c r="AX10" s="239"/>
+      <c r="AY10" s="239"/>
+      <c r="AZ10" s="239"/>
+      <c r="BA10" s="239"/>
+      <c r="BB10" s="239"/>
+      <c r="BC10" s="239"/>
     </row>
     <row r="11" spans="1:55" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="94"/>
       <c r="B11" s="5"/>
-      <c r="C11" s="221"/>
-      <c r="D11" s="222"/>
-      <c r="E11" s="222"/>
-      <c r="F11" s="222"/>
-      <c r="G11" s="222"/>
-      <c r="H11" s="222"/>
-      <c r="I11" s="222"/>
-      <c r="J11" s="222"/>
-      <c r="K11" s="222"/>
-      <c r="L11" s="222"/>
-      <c r="M11" s="222"/>
-      <c r="N11" s="222"/>
-      <c r="O11" s="222"/>
-      <c r="P11" s="222"/>
-      <c r="Q11" s="222"/>
-      <c r="R11" s="222"/>
-      <c r="S11" s="222"/>
-      <c r="T11" s="222"/>
-      <c r="U11" s="223"/>
+      <c r="C11" s="218"/>
+      <c r="D11" s="219"/>
+      <c r="E11" s="219"/>
+      <c r="F11" s="219"/>
+      <c r="G11" s="219"/>
+      <c r="H11" s="219"/>
+      <c r="I11" s="219"/>
+      <c r="J11" s="219"/>
+      <c r="K11" s="219"/>
+      <c r="L11" s="219"/>
+      <c r="M11" s="219"/>
+      <c r="N11" s="219"/>
+      <c r="O11" s="219"/>
+      <c r="P11" s="219"/>
+      <c r="Q11" s="219"/>
+      <c r="R11" s="219"/>
+      <c r="S11" s="219"/>
+      <c r="T11" s="219"/>
+      <c r="U11" s="220"/>
       <c r="V11" s="16"/>
-      <c r="X11" s="243"/>
-      <c r="Y11" s="243"/>
-      <c r="Z11" s="243"/>
-      <c r="AA11" s="243"/>
-      <c r="AB11" s="243"/>
-      <c r="AC11" s="243"/>
-      <c r="AD11" s="217"/>
-      <c r="AE11" s="217"/>
-      <c r="AF11" s="217"/>
-      <c r="AG11" s="217"/>
-      <c r="AH11" s="217"/>
-      <c r="AI11" s="217"/>
-      <c r="AJ11" s="217"/>
-      <c r="AK11" s="250"/>
-      <c r="AL11" s="250"/>
-      <c r="AM11" s="252"/>
+      <c r="X11" s="240"/>
+      <c r="Y11" s="240"/>
+      <c r="Z11" s="240"/>
+      <c r="AA11" s="240"/>
+      <c r="AB11" s="240"/>
+      <c r="AC11" s="240"/>
+      <c r="AD11" s="214"/>
+      <c r="AE11" s="214"/>
+      <c r="AF11" s="214"/>
+      <c r="AG11" s="214"/>
+      <c r="AH11" s="214"/>
+      <c r="AI11" s="214"/>
+      <c r="AJ11" s="214"/>
+      <c r="AK11" s="247"/>
+      <c r="AL11" s="247"/>
+      <c r="AM11" s="249"/>
       <c r="AN11" s="14"/>
       <c r="AQ11" s="94"/>
       <c r="AR11" s="94"/>
@@ -3169,25 +3165,25 @@
     <row r="12" spans="1:55" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="94"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="221"/>
-      <c r="D12" s="222"/>
-      <c r="E12" s="222"/>
-      <c r="F12" s="222"/>
-      <c r="G12" s="222"/>
-      <c r="H12" s="222"/>
-      <c r="I12" s="222"/>
-      <c r="J12" s="222"/>
-      <c r="K12" s="222"/>
-      <c r="L12" s="222"/>
-      <c r="M12" s="222"/>
-      <c r="N12" s="222"/>
-      <c r="O12" s="222"/>
-      <c r="P12" s="222"/>
-      <c r="Q12" s="222"/>
-      <c r="R12" s="222"/>
-      <c r="S12" s="222"/>
-      <c r="T12" s="222"/>
-      <c r="U12" s="223"/>
+      <c r="C12" s="218"/>
+      <c r="D12" s="219"/>
+      <c r="E12" s="219"/>
+      <c r="F12" s="219"/>
+      <c r="G12" s="219"/>
+      <c r="H12" s="219"/>
+      <c r="I12" s="219"/>
+      <c r="J12" s="219"/>
+      <c r="K12" s="219"/>
+      <c r="L12" s="219"/>
+      <c r="M12" s="219"/>
+      <c r="N12" s="219"/>
+      <c r="O12" s="219"/>
+      <c r="P12" s="219"/>
+      <c r="Q12" s="219"/>
+      <c r="R12" s="219"/>
+      <c r="S12" s="219"/>
+      <c r="T12" s="219"/>
+      <c r="U12" s="220"/>
       <c r="V12" s="16"/>
       <c r="AN12" s="14"/>
       <c r="AQ12" s="94"/>
@@ -3207,41 +3203,41 @@
     <row r="13" spans="1:55" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="94"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="221"/>
-      <c r="D13" s="222"/>
-      <c r="E13" s="222"/>
-      <c r="F13" s="222"/>
-      <c r="G13" s="222"/>
-      <c r="H13" s="222"/>
-      <c r="I13" s="222"/>
-      <c r="J13" s="222"/>
-      <c r="K13" s="222"/>
-      <c r="L13" s="222"/>
-      <c r="M13" s="222"/>
-      <c r="N13" s="222"/>
-      <c r="O13" s="222"/>
-      <c r="P13" s="222"/>
-      <c r="Q13" s="222"/>
-      <c r="R13" s="222"/>
-      <c r="S13" s="222"/>
-      <c r="T13" s="222"/>
-      <c r="U13" s="223"/>
+      <c r="C13" s="218"/>
+      <c r="D13" s="219"/>
+      <c r="E13" s="219"/>
+      <c r="F13" s="219"/>
+      <c r="G13" s="219"/>
+      <c r="H13" s="219"/>
+      <c r="I13" s="219"/>
+      <c r="J13" s="219"/>
+      <c r="K13" s="219"/>
+      <c r="L13" s="219"/>
+      <c r="M13" s="219"/>
+      <c r="N13" s="219"/>
+      <c r="O13" s="219"/>
+      <c r="P13" s="219"/>
+      <c r="Q13" s="219"/>
+      <c r="R13" s="219"/>
+      <c r="S13" s="219"/>
+      <c r="T13" s="219"/>
+      <c r="U13" s="220"/>
       <c r="V13" s="16"/>
-      <c r="X13" s="137" t="s">
+      <c r="X13" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="Y13" s="137"/>
-      <c r="Z13" s="137"/>
-      <c r="AA13" s="137"/>
-      <c r="AB13" s="137"/>
-      <c r="AC13" s="137"/>
-      <c r="AG13" s="232"/>
-      <c r="AH13" s="232"/>
-      <c r="AI13" s="154"/>
-      <c r="AJ13" s="154"/>
-      <c r="AK13" s="154"/>
-      <c r="AL13" s="154"/>
-      <c r="AM13" s="154"/>
+      <c r="Y13" s="134"/>
+      <c r="Z13" s="134"/>
+      <c r="AA13" s="134"/>
+      <c r="AB13" s="134"/>
+      <c r="AC13" s="134"/>
+      <c r="AG13" s="229"/>
+      <c r="AH13" s="229"/>
+      <c r="AI13" s="151"/>
+      <c r="AJ13" s="151"/>
+      <c r="AK13" s="151"/>
+      <c r="AL13" s="151"/>
+      <c r="AM13" s="151"/>
       <c r="AN13" s="14"/>
       <c r="AQ13" s="94" t="s">
         <v>8</v>
@@ -3262,25 +3258,25 @@
     <row r="14" spans="1:55" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="94"/>
       <c r="B14" s="5"/>
-      <c r="C14" s="221"/>
-      <c r="D14" s="222"/>
-      <c r="E14" s="222"/>
-      <c r="F14" s="222"/>
-      <c r="G14" s="222"/>
-      <c r="H14" s="222"/>
-      <c r="I14" s="222"/>
-      <c r="J14" s="222"/>
-      <c r="K14" s="222"/>
-      <c r="L14" s="222"/>
-      <c r="M14" s="222"/>
-      <c r="N14" s="222"/>
-      <c r="O14" s="222"/>
-      <c r="P14" s="222"/>
-      <c r="Q14" s="222"/>
-      <c r="R14" s="222"/>
-      <c r="S14" s="222"/>
-      <c r="T14" s="222"/>
-      <c r="U14" s="223"/>
+      <c r="C14" s="218"/>
+      <c r="D14" s="219"/>
+      <c r="E14" s="219"/>
+      <c r="F14" s="219"/>
+      <c r="G14" s="219"/>
+      <c r="H14" s="219"/>
+      <c r="I14" s="219"/>
+      <c r="J14" s="219"/>
+      <c r="K14" s="219"/>
+      <c r="L14" s="219"/>
+      <c r="M14" s="219"/>
+      <c r="N14" s="219"/>
+      <c r="O14" s="219"/>
+      <c r="P14" s="219"/>
+      <c r="Q14" s="219"/>
+      <c r="R14" s="219"/>
+      <c r="S14" s="219"/>
+      <c r="T14" s="219"/>
+      <c r="U14" s="220"/>
       <c r="V14" s="16"/>
       <c r="W14" s="21"/>
       <c r="AN14" s="22"/>
@@ -3303,46 +3299,46 @@
     <row r="15" spans="1:55" ht="13.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="94"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="224"/>
-      <c r="D15" s="225"/>
-      <c r="E15" s="225"/>
-      <c r="F15" s="225"/>
-      <c r="G15" s="225"/>
-      <c r="H15" s="225"/>
-      <c r="I15" s="225"/>
-      <c r="J15" s="225"/>
-      <c r="K15" s="225"/>
-      <c r="L15" s="225"/>
-      <c r="M15" s="225"/>
-      <c r="N15" s="225"/>
-      <c r="O15" s="225"/>
-      <c r="P15" s="225"/>
-      <c r="Q15" s="225"/>
-      <c r="R15" s="225"/>
-      <c r="S15" s="225"/>
-      <c r="T15" s="225"/>
-      <c r="U15" s="226"/>
+      <c r="C15" s="221"/>
+      <c r="D15" s="222"/>
+      <c r="E15" s="222"/>
+      <c r="F15" s="222"/>
+      <c r="G15" s="222"/>
+      <c r="H15" s="222"/>
+      <c r="I15" s="222"/>
+      <c r="J15" s="222"/>
+      <c r="K15" s="222"/>
+      <c r="L15" s="222"/>
+      <c r="M15" s="222"/>
+      <c r="N15" s="222"/>
+      <c r="O15" s="222"/>
+      <c r="P15" s="222"/>
+      <c r="Q15" s="222"/>
+      <c r="R15" s="222"/>
+      <c r="S15" s="222"/>
+      <c r="T15" s="222"/>
+      <c r="U15" s="223"/>
       <c r="V15" s="16"/>
       <c r="W15" s="21"/>
-      <c r="X15" s="179" t="s">
+      <c r="X15" s="176" t="s">
         <v>9</v>
       </c>
-      <c r="Y15" s="179"/>
-      <c r="Z15" s="179"/>
-      <c r="AA15" s="179"/>
-      <c r="AB15" s="179"/>
-      <c r="AC15" s="179"/>
-      <c r="AD15" s="179"/>
-      <c r="AE15" s="179"/>
-      <c r="AF15" s="179"/>
-      <c r="AG15" s="179"/>
-      <c r="AH15" s="179"/>
-      <c r="AI15" s="179"/>
-      <c r="AJ15" s="179"/>
-      <c r="AK15" s="246"/>
-      <c r="AL15" s="246"/>
-      <c r="AM15" s="246"/>
-      <c r="AN15" s="247"/>
+      <c r="Y15" s="176"/>
+      <c r="Z15" s="176"/>
+      <c r="AA15" s="176"/>
+      <c r="AB15" s="176"/>
+      <c r="AC15" s="176"/>
+      <c r="AD15" s="176"/>
+      <c r="AE15" s="176"/>
+      <c r="AF15" s="176"/>
+      <c r="AG15" s="176"/>
+      <c r="AH15" s="176"/>
+      <c r="AI15" s="176"/>
+      <c r="AJ15" s="176"/>
+      <c r="AK15" s="243"/>
+      <c r="AL15" s="243"/>
+      <c r="AM15" s="243"/>
+      <c r="AN15" s="244"/>
       <c r="AO15" s="23"/>
       <c r="AP15" s="23"/>
       <c r="AQ15" s="94" t="s">
@@ -3417,31 +3413,31 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="152"/>
-      <c r="H17" s="152"/>
-      <c r="I17" s="152"/>
-      <c r="J17" s="152"/>
-      <c r="K17" s="152"/>
-      <c r="L17" s="152"/>
-      <c r="M17" s="152"/>
-      <c r="N17" s="152"/>
-      <c r="O17" s="152"/>
-      <c r="P17" s="152"/>
-      <c r="Q17" s="152"/>
-      <c r="R17" s="152"/>
-      <c r="S17" s="152"/>
-      <c r="T17" s="152"/>
-      <c r="U17" s="152"/>
+      <c r="G17" s="149"/>
+      <c r="H17" s="149"/>
+      <c r="I17" s="149"/>
+      <c r="J17" s="149"/>
+      <c r="K17" s="149"/>
+      <c r="L17" s="149"/>
+      <c r="M17" s="149"/>
+      <c r="N17" s="149"/>
+      <c r="O17" s="149"/>
+      <c r="P17" s="149"/>
+      <c r="Q17" s="149"/>
+      <c r="R17" s="149"/>
+      <c r="S17" s="149"/>
+      <c r="T17" s="149"/>
+      <c r="U17" s="149"/>
       <c r="V17" s="16"/>
       <c r="W17" s="24"/>
       <c r="AN17" s="18"/>
     </row>
     <row r="18" spans="1:49" ht="5.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="147" t="s">
+      <c r="A18" s="144" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="5"/>
-      <c r="C18" s="227"/>
+      <c r="C18" s="224"/>
       <c r="D18" s="116" t="s">
         <v>15</v>
       </c>
@@ -3464,29 +3460,29 @@
       <c r="U18" s="118"/>
       <c r="V18" s="16"/>
       <c r="W18" s="24"/>
-      <c r="X18" s="181"/>
-      <c r="Y18" s="139"/>
-      <c r="Z18" s="150" t="s">
+      <c r="X18" s="178"/>
+      <c r="Y18" s="136"/>
+      <c r="Z18" s="147" t="s">
         <v>16</v>
       </c>
-      <c r="AA18" s="150"/>
-      <c r="AB18" s="150"/>
-      <c r="AC18" s="150"/>
-      <c r="AD18" s="150"/>
-      <c r="AE18" s="150"/>
-      <c r="AF18" s="150"/>
-      <c r="AG18" s="150"/>
-      <c r="AH18" s="150"/>
-      <c r="AI18" s="150"/>
-      <c r="AJ18" s="150"/>
-      <c r="AK18" s="150"/>
-      <c r="AL18" s="150"/>
+      <c r="AA18" s="147"/>
+      <c r="AB18" s="147"/>
+      <c r="AC18" s="147"/>
+      <c r="AD18" s="147"/>
+      <c r="AE18" s="147"/>
+      <c r="AF18" s="147"/>
+      <c r="AG18" s="147"/>
+      <c r="AH18" s="147"/>
+      <c r="AI18" s="147"/>
+      <c r="AJ18" s="147"/>
+      <c r="AK18" s="147"/>
+      <c r="AL18" s="147"/>
       <c r="AN18" s="18"/>
     </row>
     <row r="19" spans="1:49" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="147"/>
+      <c r="A19" s="144"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="228"/>
+      <c r="C19" s="225"/>
       <c r="D19" s="116"/>
       <c r="E19" s="117"/>
       <c r="F19" s="117"/>
@@ -3507,25 +3503,25 @@
       <c r="U19" s="118"/>
       <c r="V19" s="16"/>
       <c r="W19" s="24"/>
-      <c r="X19" s="182"/>
-      <c r="Y19" s="139"/>
-      <c r="Z19" s="150"/>
-      <c r="AA19" s="150"/>
-      <c r="AB19" s="150"/>
-      <c r="AC19" s="150"/>
-      <c r="AD19" s="150"/>
-      <c r="AE19" s="150"/>
-      <c r="AF19" s="150"/>
-      <c r="AG19" s="150"/>
-      <c r="AH19" s="150"/>
-      <c r="AI19" s="150"/>
-      <c r="AJ19" s="150"/>
-      <c r="AK19" s="150"/>
-      <c r="AL19" s="150"/>
+      <c r="X19" s="179"/>
+      <c r="Y19" s="136"/>
+      <c r="Z19" s="147"/>
+      <c r="AA19" s="147"/>
+      <c r="AB19" s="147"/>
+      <c r="AC19" s="147"/>
+      <c r="AD19" s="147"/>
+      <c r="AE19" s="147"/>
+      <c r="AF19" s="147"/>
+      <c r="AG19" s="147"/>
+      <c r="AH19" s="147"/>
+      <c r="AI19" s="147"/>
+      <c r="AJ19" s="147"/>
+      <c r="AK19" s="147"/>
+      <c r="AL19" s="147"/>
       <c r="AN19" s="18"/>
     </row>
     <row r="20" spans="1:49" ht="5.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="147"/>
+      <c r="A20" s="144"/>
       <c r="B20" s="5"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -3550,19 +3546,19 @@
       <c r="W20" s="24"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
-      <c r="Z20" s="150"/>
-      <c r="AA20" s="150"/>
-      <c r="AB20" s="150"/>
-      <c r="AC20" s="150"/>
-      <c r="AD20" s="150"/>
-      <c r="AE20" s="150"/>
-      <c r="AF20" s="150"/>
-      <c r="AG20" s="150"/>
-      <c r="AH20" s="150"/>
-      <c r="AI20" s="150"/>
-      <c r="AJ20" s="150"/>
-      <c r="AK20" s="150"/>
-      <c r="AL20" s="150"/>
+      <c r="Z20" s="147"/>
+      <c r="AA20" s="147"/>
+      <c r="AB20" s="147"/>
+      <c r="AC20" s="147"/>
+      <c r="AD20" s="147"/>
+      <c r="AE20" s="147"/>
+      <c r="AF20" s="147"/>
+      <c r="AG20" s="147"/>
+      <c r="AH20" s="147"/>
+      <c r="AI20" s="147"/>
+      <c r="AJ20" s="147"/>
+      <c r="AK20" s="147"/>
+      <c r="AL20" s="147"/>
       <c r="AN20" s="18"/>
     </row>
     <row r="21" spans="1:49" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3635,22 +3631,22 @@
       <c r="U22" s="17"/>
       <c r="V22" s="16"/>
       <c r="W22" s="24"/>
-      <c r="X22" s="177"/>
-      <c r="Y22" s="177"/>
-      <c r="Z22" s="177"/>
-      <c r="AA22" s="177"/>
-      <c r="AB22" s="177"/>
-      <c r="AC22" s="177"/>
-      <c r="AD22" s="177"/>
-      <c r="AE22" s="177"/>
-      <c r="AF22" s="177"/>
-      <c r="AG22" s="177"/>
-      <c r="AH22" s="177"/>
-      <c r="AI22" s="177"/>
-      <c r="AJ22" s="177"/>
-      <c r="AK22" s="177"/>
-      <c r="AL22" s="177"/>
-      <c r="AM22" s="177"/>
+      <c r="X22" s="174"/>
+      <c r="Y22" s="174"/>
+      <c r="Z22" s="174"/>
+      <c r="AA22" s="174"/>
+      <c r="AB22" s="174"/>
+      <c r="AC22" s="174"/>
+      <c r="AD22" s="174"/>
+      <c r="AE22" s="174"/>
+      <c r="AF22" s="174"/>
+      <c r="AG22" s="174"/>
+      <c r="AH22" s="174"/>
+      <c r="AI22" s="174"/>
+      <c r="AJ22" s="174"/>
+      <c r="AK22" s="174"/>
+      <c r="AL22" s="174"/>
+      <c r="AM22" s="174"/>
       <c r="AN22" s="18"/>
       <c r="AW22" s="6"/>
     </row>
@@ -3669,59 +3665,59 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="139"/>
-      <c r="L23" s="139"/>
-      <c r="M23" s="139"/>
-      <c r="N23" s="139"/>
-      <c r="O23" s="139"/>
-      <c r="P23" s="139"/>
-      <c r="Q23" s="139"/>
-      <c r="R23" s="139"/>
-      <c r="S23" s="139"/>
-      <c r="T23" s="139"/>
-      <c r="U23" s="139"/>
+      <c r="K23" s="136"/>
+      <c r="L23" s="136"/>
+      <c r="M23" s="136"/>
+      <c r="N23" s="136"/>
+      <c r="O23" s="136"/>
+      <c r="P23" s="136"/>
+      <c r="Q23" s="136"/>
+      <c r="R23" s="136"/>
+      <c r="S23" s="136"/>
+      <c r="T23" s="136"/>
+      <c r="U23" s="136"/>
       <c r="V23" s="81"/>
       <c r="W23" s="82"/>
-      <c r="X23" s="178"/>
-      <c r="Y23" s="178"/>
-      <c r="Z23" s="178"/>
-      <c r="AA23" s="178"/>
-      <c r="AB23" s="178"/>
-      <c r="AC23" s="178"/>
-      <c r="AD23" s="178"/>
-      <c r="AE23" s="178"/>
-      <c r="AF23" s="178"/>
-      <c r="AG23" s="178"/>
-      <c r="AH23" s="178"/>
-      <c r="AI23" s="178"/>
-      <c r="AJ23" s="178"/>
-      <c r="AK23" s="178"/>
-      <c r="AL23" s="178"/>
-      <c r="AM23" s="178"/>
+      <c r="X23" s="175"/>
+      <c r="Y23" s="175"/>
+      <c r="Z23" s="175"/>
+      <c r="AA23" s="175"/>
+      <c r="AB23" s="175"/>
+      <c r="AC23" s="175"/>
+      <c r="AD23" s="175"/>
+      <c r="AE23" s="175"/>
+      <c r="AF23" s="175"/>
+      <c r="AG23" s="175"/>
+      <c r="AH23" s="175"/>
+      <c r="AI23" s="175"/>
+      <c r="AJ23" s="175"/>
+      <c r="AK23" s="175"/>
+      <c r="AL23" s="175"/>
+      <c r="AM23" s="175"/>
       <c r="AN23" s="18"/>
       <c r="AW23" s="6"/>
     </row>
     <row r="24" spans="1:49" ht="5.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="94"/>
       <c r="B24" s="27"/>
-      <c r="C24" s="176"/>
-      <c r="D24" s="176"/>
-      <c r="E24" s="176"/>
-      <c r="F24" s="176"/>
-      <c r="G24" s="176"/>
-      <c r="H24" s="176"/>
-      <c r="I24" s="176"/>
-      <c r="J24" s="176"/>
-      <c r="K24" s="180"/>
-      <c r="L24" s="180"/>
-      <c r="M24" s="180"/>
-      <c r="N24" s="180"/>
-      <c r="O24" s="180"/>
-      <c r="P24" s="180"/>
-      <c r="Q24" s="180"/>
-      <c r="R24" s="180"/>
-      <c r="S24" s="180"/>
-      <c r="T24" s="180"/>
+      <c r="C24" s="173"/>
+      <c r="D24" s="173"/>
+      <c r="E24" s="173"/>
+      <c r="F24" s="173"/>
+      <c r="G24" s="173"/>
+      <c r="H24" s="173"/>
+      <c r="I24" s="173"/>
+      <c r="J24" s="173"/>
+      <c r="K24" s="177"/>
+      <c r="L24" s="177"/>
+      <c r="M24" s="177"/>
+      <c r="N24" s="177"/>
+      <c r="O24" s="177"/>
+      <c r="P24" s="177"/>
+      <c r="Q24" s="177"/>
+      <c r="R24" s="177"/>
+      <c r="S24" s="177"/>
+      <c r="T24" s="177"/>
       <c r="U24" s="19"/>
       <c r="V24" s="28"/>
       <c r="W24" s="29"/>
@@ -3792,25 +3788,25 @@
       <c r="D26" s="126"/>
       <c r="E26" s="126"/>
       <c r="F26" s="126"/>
-      <c r="G26" s="153"/>
-      <c r="H26" s="154"/>
-      <c r="I26" s="154"/>
-      <c r="J26" s="154"/>
-      <c r="K26" s="154"/>
-      <c r="L26" s="154"/>
-      <c r="M26" s="154"/>
+      <c r="G26" s="150"/>
+      <c r="H26" s="151"/>
+      <c r="I26" s="151"/>
+      <c r="J26" s="151"/>
+      <c r="K26" s="151"/>
+      <c r="L26" s="151"/>
+      <c r="M26" s="151"/>
       <c r="O26" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="P26" s="141"/>
-      <c r="Q26" s="171"/>
-      <c r="R26" s="171"/>
-      <c r="S26" s="171"/>
+      <c r="P26" s="138"/>
+      <c r="Q26" s="168"/>
+      <c r="R26" s="168"/>
+      <c r="S26" s="168"/>
       <c r="T26" s="36"/>
-      <c r="U26" s="135" t="s">
+      <c r="U26" s="132" t="s">
         <v>24</v>
       </c>
-      <c r="V26" s="144"/>
+      <c r="V26" s="141"/>
       <c r="W26" s="127"/>
       <c r="X26" s="127"/>
       <c r="Y26" s="127"/>
@@ -3826,7 +3822,7 @@
       <c r="AW26" s="6"/>
     </row>
     <row r="27" spans="1:49" ht="5.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="148" t="s">
+      <c r="A27" s="145" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="5"/>
@@ -3835,7 +3831,7 @@
       <c r="AW27" s="6"/>
     </row>
     <row r="28" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="148"/>
+      <c r="A28" s="145"/>
       <c r="B28" s="5"/>
       <c r="C28" s="69" t="s">
         <v>27</v>
@@ -3873,9 +3869,9 @@
       <c r="AJ28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AL28" s="160"/>
-      <c r="AM28" s="160"/>
-      <c r="AN28" s="161"/>
+      <c r="AL28" s="157"/>
+      <c r="AM28" s="157"/>
+      <c r="AN28" s="158"/>
       <c r="AW28" s="6"/>
     </row>
     <row r="29" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3883,33 +3879,33 @@
         <v>30</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="C29" s="140"/>
-      <c r="D29" s="140"/>
-      <c r="E29" s="140"/>
-      <c r="F29" s="140"/>
-      <c r="G29" s="140"/>
-      <c r="H29" s="140"/>
-      <c r="I29" s="140"/>
-      <c r="J29" s="140"/>
-      <c r="K29" s="140"/>
+      <c r="C29" s="137"/>
+      <c r="D29" s="137"/>
+      <c r="E29" s="137"/>
+      <c r="F29" s="137"/>
+      <c r="G29" s="137"/>
+      <c r="H29" s="137"/>
+      <c r="I29" s="137"/>
+      <c r="J29" s="137"/>
+      <c r="K29" s="137"/>
       <c r="L29" s="24"/>
-      <c r="M29" s="149"/>
-      <c r="N29" s="149"/>
-      <c r="O29" s="149"/>
-      <c r="P29" s="149"/>
-      <c r="Q29" s="149"/>
-      <c r="R29" s="149"/>
-      <c r="S29" s="149"/>
-      <c r="T29" s="149"/>
-      <c r="U29" s="149"/>
-      <c r="V29" s="149"/>
-      <c r="W29" s="149"/>
-      <c r="X29" s="149"/>
-      <c r="Y29" s="149"/>
-      <c r="Z29" s="149"/>
-      <c r="AA29" s="149"/>
-      <c r="AB29" s="149"/>
-      <c r="AC29" s="149"/>
+      <c r="M29" s="146"/>
+      <c r="N29" s="146"/>
+      <c r="O29" s="146"/>
+      <c r="P29" s="146"/>
+      <c r="Q29" s="146"/>
+      <c r="R29" s="146"/>
+      <c r="S29" s="146"/>
+      <c r="T29" s="146"/>
+      <c r="U29" s="146"/>
+      <c r="V29" s="146"/>
+      <c r="W29" s="146"/>
+      <c r="X29" s="146"/>
+      <c r="Y29" s="146"/>
+      <c r="Z29" s="146"/>
+      <c r="AA29" s="146"/>
+      <c r="AB29" s="146"/>
+      <c r="AC29" s="146"/>
       <c r="AG29" s="37"/>
       <c r="AN29" s="18"/>
       <c r="AW29" s="38" t="s">
@@ -3919,41 +3915,41 @@
     <row r="30" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="97"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="143"/>
-      <c r="D30" s="143"/>
-      <c r="E30" s="143"/>
-      <c r="F30" s="143"/>
-      <c r="G30" s="143"/>
-      <c r="H30" s="143"/>
-      <c r="I30" s="143"/>
-      <c r="J30" s="143"/>
-      <c r="K30" s="143"/>
-      <c r="L30" s="143"/>
-      <c r="M30" s="143"/>
-      <c r="N30" s="143"/>
-      <c r="O30" s="143"/>
-      <c r="P30" s="143"/>
-      <c r="Q30" s="143"/>
-      <c r="R30" s="143"/>
-      <c r="S30" s="143"/>
-      <c r="T30" s="143"/>
-      <c r="U30" s="143"/>
-      <c r="V30" s="143"/>
-      <c r="W30" s="143"/>
-      <c r="X30" s="143"/>
-      <c r="Y30" s="143"/>
-      <c r="Z30" s="143"/>
-      <c r="AA30" s="143"/>
-      <c r="AB30" s="143"/>
-      <c r="AC30" s="143"/>
+      <c r="C30" s="140"/>
+      <c r="D30" s="140"/>
+      <c r="E30" s="140"/>
+      <c r="F30" s="140"/>
+      <c r="G30" s="140"/>
+      <c r="H30" s="140"/>
+      <c r="I30" s="140"/>
+      <c r="J30" s="140"/>
+      <c r="K30" s="140"/>
+      <c r="L30" s="140"/>
+      <c r="M30" s="140"/>
+      <c r="N30" s="140"/>
+      <c r="O30" s="140"/>
+      <c r="P30" s="140"/>
+      <c r="Q30" s="140"/>
+      <c r="R30" s="140"/>
+      <c r="S30" s="140"/>
+      <c r="T30" s="140"/>
+      <c r="U30" s="140"/>
+      <c r="V30" s="140"/>
+      <c r="W30" s="140"/>
+      <c r="X30" s="140"/>
+      <c r="Y30" s="140"/>
+      <c r="Z30" s="140"/>
+      <c r="AA30" s="140"/>
+      <c r="AB30" s="140"/>
+      <c r="AC30" s="140"/>
       <c r="AE30" s="36"/>
       <c r="AG30" s="37"/>
       <c r="AJ30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AL30" s="160"/>
-      <c r="AM30" s="160"/>
-      <c r="AN30" s="161"/>
+      <c r="AL30" s="157"/>
+      <c r="AM30" s="157"/>
+      <c r="AN30" s="158"/>
       <c r="AW30" s="38" t="s">
         <v>33</v>
       </c>
@@ -3963,19 +3959,19 @@
         <v>34</v>
       </c>
       <c r="B31" s="5"/>
-      <c r="C31" s="151" t="s">
+      <c r="C31" s="148" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="151"/>
-      <c r="E31" s="151"/>
-      <c r="F31" s="151"/>
-      <c r="G31" s="151"/>
-      <c r="H31" s="151"/>
-      <c r="I31" s="151"/>
-      <c r="J31" s="151"/>
-      <c r="K31" s="151"/>
-      <c r="L31" s="151"/>
-      <c r="M31" s="151"/>
+      <c r="D31" s="148"/>
+      <c r="E31" s="148"/>
+      <c r="F31" s="148"/>
+      <c r="G31" s="148"/>
+      <c r="H31" s="148"/>
+      <c r="I31" s="148"/>
+      <c r="J31" s="148"/>
+      <c r="K31" s="148"/>
+      <c r="L31" s="148"/>
+      <c r="M31" s="148"/>
       <c r="N31" s="70"/>
       <c r="O31" s="70"/>
       <c r="P31" s="70"/>
@@ -4003,45 +3999,45 @@
     <row r="32" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="94"/>
       <c r="B32" s="5"/>
-      <c r="C32" s="202"/>
-      <c r="D32" s="192"/>
-      <c r="E32" s="192"/>
-      <c r="F32" s="192"/>
-      <c r="G32" s="192"/>
-      <c r="H32" s="192"/>
-      <c r="I32" s="192"/>
-      <c r="J32" s="192"/>
-      <c r="K32" s="192"/>
-      <c r="L32" s="192"/>
-      <c r="M32" s="192"/>
-      <c r="N32" s="192"/>
-      <c r="O32" s="192"/>
-      <c r="P32" s="192"/>
-      <c r="Q32" s="192"/>
-      <c r="R32" s="192"/>
-      <c r="S32" s="192"/>
-      <c r="T32" s="192"/>
-      <c r="U32" s="192"/>
-      <c r="V32" s="192"/>
-      <c r="W32" s="192"/>
-      <c r="X32" s="192"/>
-      <c r="Y32" s="192"/>
-      <c r="Z32" s="192"/>
-      <c r="AA32" s="192"/>
-      <c r="AB32" s="192"/>
-      <c r="AC32" s="193"/>
+      <c r="C32" s="199"/>
+      <c r="D32" s="189"/>
+      <c r="E32" s="189"/>
+      <c r="F32" s="189"/>
+      <c r="G32" s="189"/>
+      <c r="H32" s="189"/>
+      <c r="I32" s="189"/>
+      <c r="J32" s="189"/>
+      <c r="K32" s="189"/>
+      <c r="L32" s="189"/>
+      <c r="M32" s="189"/>
+      <c r="N32" s="189"/>
+      <c r="O32" s="189"/>
+      <c r="P32" s="189"/>
+      <c r="Q32" s="189"/>
+      <c r="R32" s="189"/>
+      <c r="S32" s="189"/>
+      <c r="T32" s="189"/>
+      <c r="U32" s="189"/>
+      <c r="V32" s="189"/>
+      <c r="W32" s="189"/>
+      <c r="X32" s="189"/>
+      <c r="Y32" s="189"/>
+      <c r="Z32" s="189"/>
+      <c r="AA32" s="189"/>
+      <c r="AB32" s="189"/>
+      <c r="AC32" s="190"/>
       <c r="AD32" s="71"/>
       <c r="AE32" s="20"/>
       <c r="AG32" s="37"/>
       <c r="AJ32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AL32" s="183">
+      <c r="AL32" s="180">
         <f>AL28+AL30</f>
         <v>0</v>
       </c>
-      <c r="AM32" s="183"/>
-      <c r="AN32" s="184"/>
+      <c r="AM32" s="180"/>
+      <c r="AN32" s="181"/>
       <c r="AW32" s="38" t="s">
         <v>38</v>
       </c>
@@ -4049,33 +4045,33 @@
     <row r="33" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="94"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="194"/>
-      <c r="D33" s="195"/>
-      <c r="E33" s="195"/>
-      <c r="F33" s="195"/>
-      <c r="G33" s="195"/>
-      <c r="H33" s="195"/>
-      <c r="I33" s="195"/>
-      <c r="J33" s="195"/>
-      <c r="K33" s="195"/>
-      <c r="L33" s="195"/>
-      <c r="M33" s="195"/>
-      <c r="N33" s="195"/>
-      <c r="O33" s="195"/>
-      <c r="P33" s="195"/>
-      <c r="Q33" s="195"/>
-      <c r="R33" s="195"/>
-      <c r="S33" s="195"/>
-      <c r="T33" s="195"/>
-      <c r="U33" s="195"/>
-      <c r="V33" s="195"/>
-      <c r="W33" s="195"/>
-      <c r="X33" s="195"/>
-      <c r="Y33" s="195"/>
-      <c r="Z33" s="195"/>
-      <c r="AA33" s="195"/>
-      <c r="AB33" s="195"/>
-      <c r="AC33" s="196"/>
+      <c r="C33" s="191"/>
+      <c r="D33" s="192"/>
+      <c r="E33" s="192"/>
+      <c r="F33" s="192"/>
+      <c r="G33" s="192"/>
+      <c r="H33" s="192"/>
+      <c r="I33" s="192"/>
+      <c r="J33" s="192"/>
+      <c r="K33" s="192"/>
+      <c r="L33" s="192"/>
+      <c r="M33" s="192"/>
+      <c r="N33" s="192"/>
+      <c r="O33" s="192"/>
+      <c r="P33" s="192"/>
+      <c r="Q33" s="192"/>
+      <c r="R33" s="192"/>
+      <c r="S33" s="192"/>
+      <c r="T33" s="192"/>
+      <c r="U33" s="192"/>
+      <c r="V33" s="192"/>
+      <c r="W33" s="192"/>
+      <c r="X33" s="192"/>
+      <c r="Y33" s="192"/>
+      <c r="Z33" s="192"/>
+      <c r="AA33" s="192"/>
+      <c r="AB33" s="192"/>
+      <c r="AC33" s="193"/>
       <c r="AD33" s="39"/>
       <c r="AE33" s="26"/>
       <c r="AG33" s="37"/>
@@ -4089,74 +4085,74 @@
     <row r="34" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="94"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="194"/>
-      <c r="D34" s="195"/>
-      <c r="E34" s="195"/>
-      <c r="F34" s="195"/>
-      <c r="G34" s="195"/>
-      <c r="H34" s="195"/>
-      <c r="I34" s="195"/>
-      <c r="J34" s="195"/>
-      <c r="K34" s="195"/>
-      <c r="L34" s="195"/>
-      <c r="M34" s="195"/>
-      <c r="N34" s="195"/>
-      <c r="O34" s="195"/>
-      <c r="P34" s="195"/>
-      <c r="Q34" s="195"/>
-      <c r="R34" s="195"/>
-      <c r="S34" s="195"/>
-      <c r="T34" s="195"/>
-      <c r="U34" s="195"/>
-      <c r="V34" s="195"/>
-      <c r="W34" s="195"/>
-      <c r="X34" s="195"/>
-      <c r="Y34" s="195"/>
-      <c r="Z34" s="195"/>
-      <c r="AA34" s="195"/>
-      <c r="AB34" s="195"/>
-      <c r="AC34" s="196"/>
+      <c r="C34" s="191"/>
+      <c r="D34" s="192"/>
+      <c r="E34" s="192"/>
+      <c r="F34" s="192"/>
+      <c r="G34" s="192"/>
+      <c r="H34" s="192"/>
+      <c r="I34" s="192"/>
+      <c r="J34" s="192"/>
+      <c r="K34" s="192"/>
+      <c r="L34" s="192"/>
+      <c r="M34" s="192"/>
+      <c r="N34" s="192"/>
+      <c r="O34" s="192"/>
+      <c r="P34" s="192"/>
+      <c r="Q34" s="192"/>
+      <c r="R34" s="192"/>
+      <c r="S34" s="192"/>
+      <c r="T34" s="192"/>
+      <c r="U34" s="192"/>
+      <c r="V34" s="192"/>
+      <c r="W34" s="192"/>
+      <c r="X34" s="192"/>
+      <c r="Y34" s="192"/>
+      <c r="Z34" s="192"/>
+      <c r="AA34" s="192"/>
+      <c r="AB34" s="192"/>
+      <c r="AC34" s="193"/>
       <c r="AD34" s="39"/>
       <c r="AE34" s="26"/>
       <c r="AG34" s="37"/>
       <c r="AJ34" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AL34" s="187"/>
-      <c r="AM34" s="187"/>
-      <c r="AN34" s="188"/>
+      <c r="AL34" s="184"/>
+      <c r="AM34" s="184"/>
+      <c r="AN34" s="185"/>
       <c r="AW34" s="38"/>
     </row>
     <row r="35" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="94"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="194"/>
-      <c r="D35" s="195"/>
-      <c r="E35" s="195"/>
-      <c r="F35" s="195"/>
-      <c r="G35" s="195"/>
-      <c r="H35" s="195"/>
-      <c r="I35" s="195"/>
-      <c r="J35" s="195"/>
-      <c r="K35" s="195"/>
-      <c r="L35" s="195"/>
-      <c r="M35" s="195"/>
-      <c r="N35" s="195"/>
-      <c r="O35" s="195"/>
-      <c r="P35" s="195"/>
-      <c r="Q35" s="195"/>
-      <c r="R35" s="195"/>
-      <c r="S35" s="195"/>
-      <c r="T35" s="195"/>
-      <c r="U35" s="195"/>
-      <c r="V35" s="195"/>
-      <c r="W35" s="195"/>
-      <c r="X35" s="195"/>
-      <c r="Y35" s="195"/>
-      <c r="Z35" s="195"/>
-      <c r="AA35" s="195"/>
-      <c r="AB35" s="195"/>
-      <c r="AC35" s="196"/>
+      <c r="C35" s="191"/>
+      <c r="D35" s="192"/>
+      <c r="E35" s="192"/>
+      <c r="F35" s="192"/>
+      <c r="G35" s="192"/>
+      <c r="H35" s="192"/>
+      <c r="I35" s="192"/>
+      <c r="J35" s="192"/>
+      <c r="K35" s="192"/>
+      <c r="L35" s="192"/>
+      <c r="M35" s="192"/>
+      <c r="N35" s="192"/>
+      <c r="O35" s="192"/>
+      <c r="P35" s="192"/>
+      <c r="Q35" s="192"/>
+      <c r="R35" s="192"/>
+      <c r="S35" s="192"/>
+      <c r="T35" s="192"/>
+      <c r="U35" s="192"/>
+      <c r="V35" s="192"/>
+      <c r="W35" s="192"/>
+      <c r="X35" s="192"/>
+      <c r="Y35" s="192"/>
+      <c r="Z35" s="192"/>
+      <c r="AA35" s="192"/>
+      <c r="AB35" s="192"/>
+      <c r="AC35" s="193"/>
       <c r="AD35" s="39"/>
       <c r="AE35" s="26"/>
       <c r="AG35" s="37"/>
@@ -4170,33 +4166,33 @@
     <row r="36" spans="1:49" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="94"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="197"/>
-      <c r="D36" s="198"/>
-      <c r="E36" s="198"/>
-      <c r="F36" s="198"/>
-      <c r="G36" s="198"/>
-      <c r="H36" s="198"/>
-      <c r="I36" s="198"/>
-      <c r="J36" s="198"/>
-      <c r="K36" s="198"/>
-      <c r="L36" s="198"/>
-      <c r="M36" s="198"/>
-      <c r="N36" s="198"/>
-      <c r="O36" s="198"/>
-      <c r="P36" s="198"/>
-      <c r="Q36" s="198"/>
-      <c r="R36" s="198"/>
-      <c r="S36" s="198"/>
-      <c r="T36" s="198"/>
-      <c r="U36" s="198"/>
-      <c r="V36" s="198"/>
-      <c r="W36" s="198"/>
-      <c r="X36" s="198"/>
-      <c r="Y36" s="198"/>
-      <c r="Z36" s="198"/>
-      <c r="AA36" s="198"/>
-      <c r="AB36" s="198"/>
-      <c r="AC36" s="199"/>
+      <c r="C36" s="194"/>
+      <c r="D36" s="195"/>
+      <c r="E36" s="195"/>
+      <c r="F36" s="195"/>
+      <c r="G36" s="195"/>
+      <c r="H36" s="195"/>
+      <c r="I36" s="195"/>
+      <c r="J36" s="195"/>
+      <c r="K36" s="195"/>
+      <c r="L36" s="195"/>
+      <c r="M36" s="195"/>
+      <c r="N36" s="195"/>
+      <c r="O36" s="195"/>
+      <c r="P36" s="195"/>
+      <c r="Q36" s="195"/>
+      <c r="R36" s="195"/>
+      <c r="S36" s="195"/>
+      <c r="T36" s="195"/>
+      <c r="U36" s="195"/>
+      <c r="V36" s="195"/>
+      <c r="W36" s="195"/>
+      <c r="X36" s="195"/>
+      <c r="Y36" s="195"/>
+      <c r="Z36" s="195"/>
+      <c r="AA36" s="195"/>
+      <c r="AB36" s="195"/>
+      <c r="AC36" s="196"/>
       <c r="AD36" s="39"/>
       <c r="AE36" s="36"/>
       <c r="AG36" s="37"/>
@@ -4204,12 +4200,12 @@
         <v>37</v>
       </c>
       <c r="AK36" s="34"/>
-      <c r="AL36" s="183">
+      <c r="AL36" s="180">
         <f>(AL30+AL28)*AL34</f>
         <v>0</v>
       </c>
-      <c r="AM36" s="183"/>
-      <c r="AN36" s="184"/>
+      <c r="AM36" s="180"/>
+      <c r="AN36" s="181"/>
       <c r="AW36" s="38" t="s">
         <v>40</v>
       </c>
@@ -4262,13 +4258,13 @@
     <row r="38" spans="1:49" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="94"/>
       <c r="B38" s="5"/>
-      <c r="C38" s="229" t="s">
+      <c r="C38" s="226" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="229"/>
-      <c r="E38" s="229"/>
-      <c r="F38" s="229"/>
-      <c r="G38" s="229"/>
+      <c r="D38" s="226"/>
+      <c r="E38" s="226"/>
+      <c r="F38" s="226"/>
+      <c r="G38" s="226"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
@@ -4307,25 +4303,25 @@
       <c r="D39" s="126"/>
       <c r="E39" s="126"/>
       <c r="F39" s="126"/>
-      <c r="G39" s="153"/>
-      <c r="H39" s="154"/>
-      <c r="I39" s="154"/>
-      <c r="J39" s="154"/>
-      <c r="K39" s="154"/>
-      <c r="L39" s="154"/>
-      <c r="M39" s="154"/>
+      <c r="G39" s="150"/>
+      <c r="H39" s="151"/>
+      <c r="I39" s="151"/>
+      <c r="J39" s="151"/>
+      <c r="K39" s="151"/>
+      <c r="L39" s="151"/>
+      <c r="M39" s="151"/>
       <c r="O39" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="P39" s="141"/>
-      <c r="Q39" s="142"/>
-      <c r="R39" s="142"/>
-      <c r="S39" s="142"/>
+      <c r="P39" s="138"/>
+      <c r="Q39" s="139"/>
+      <c r="R39" s="139"/>
+      <c r="S39" s="139"/>
       <c r="T39" s="56"/>
-      <c r="U39" s="135" t="s">
+      <c r="U39" s="132" t="s">
         <v>24</v>
       </c>
-      <c r="V39" s="144"/>
+      <c r="V39" s="141"/>
       <c r="W39" s="127"/>
       <c r="X39" s="127"/>
       <c r="Y39" s="127"/>
@@ -4341,7 +4337,7 @@
       <c r="AW39" s="6"/>
     </row>
     <row r="40" spans="1:49" ht="5.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="148" t="s">
+      <c r="A40" s="145" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="5"/>
@@ -4350,7 +4346,7 @@
       <c r="AW40" s="6"/>
     </row>
     <row r="41" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="148"/>
+      <c r="A41" s="145"/>
       <c r="B41" s="5"/>
       <c r="C41" s="69" t="s">
         <v>27</v>
@@ -4388,9 +4384,9 @@
       <c r="AJ41" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AL41" s="160"/>
-      <c r="AM41" s="160"/>
-      <c r="AN41" s="161"/>
+      <c r="AL41" s="157"/>
+      <c r="AM41" s="157"/>
+      <c r="AN41" s="158"/>
       <c r="AW41" s="6"/>
     </row>
     <row r="42" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4398,33 +4394,33 @@
         <v>30</v>
       </c>
       <c r="B42" s="5"/>
-      <c r="C42" s="140"/>
-      <c r="D42" s="140"/>
-      <c r="E42" s="140"/>
-      <c r="F42" s="140"/>
-      <c r="G42" s="140"/>
-      <c r="H42" s="140"/>
-      <c r="I42" s="140"/>
-      <c r="J42" s="140"/>
-      <c r="K42" s="140"/>
+      <c r="C42" s="137"/>
+      <c r="D42" s="137"/>
+      <c r="E42" s="137"/>
+      <c r="F42" s="137"/>
+      <c r="G42" s="137"/>
+      <c r="H42" s="137"/>
+      <c r="I42" s="137"/>
+      <c r="J42" s="137"/>
+      <c r="K42" s="137"/>
       <c r="L42" s="24"/>
-      <c r="M42" s="149"/>
-      <c r="N42" s="149"/>
-      <c r="O42" s="149"/>
-      <c r="P42" s="149"/>
-      <c r="Q42" s="149"/>
-      <c r="R42" s="149"/>
-      <c r="S42" s="149"/>
-      <c r="T42" s="149"/>
-      <c r="U42" s="149"/>
-      <c r="V42" s="149"/>
-      <c r="W42" s="149"/>
-      <c r="X42" s="149"/>
-      <c r="Y42" s="149"/>
-      <c r="Z42" s="149"/>
-      <c r="AA42" s="149"/>
-      <c r="AB42" s="149"/>
-      <c r="AC42" s="149"/>
+      <c r="M42" s="146"/>
+      <c r="N42" s="146"/>
+      <c r="O42" s="146"/>
+      <c r="P42" s="146"/>
+      <c r="Q42" s="146"/>
+      <c r="R42" s="146"/>
+      <c r="S42" s="146"/>
+      <c r="T42" s="146"/>
+      <c r="U42" s="146"/>
+      <c r="V42" s="146"/>
+      <c r="W42" s="146"/>
+      <c r="X42" s="146"/>
+      <c r="Y42" s="146"/>
+      <c r="Z42" s="146"/>
+      <c r="AA42" s="146"/>
+      <c r="AB42" s="146"/>
+      <c r="AC42" s="146"/>
       <c r="AG42" s="37"/>
       <c r="AN42" s="18"/>
       <c r="AW42" s="38" t="s">
@@ -4434,41 +4430,41 @@
     <row r="43" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="97"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="143"/>
-      <c r="D43" s="143"/>
-      <c r="E43" s="143"/>
-      <c r="F43" s="143"/>
-      <c r="G43" s="143"/>
-      <c r="H43" s="143"/>
-      <c r="I43" s="143"/>
-      <c r="J43" s="143"/>
-      <c r="K43" s="143"/>
-      <c r="L43" s="143"/>
-      <c r="M43" s="143"/>
-      <c r="N43" s="143"/>
-      <c r="O43" s="143"/>
-      <c r="P43" s="143"/>
-      <c r="Q43" s="143"/>
-      <c r="R43" s="143"/>
-      <c r="S43" s="143"/>
-      <c r="T43" s="143"/>
-      <c r="U43" s="143"/>
-      <c r="V43" s="143"/>
-      <c r="W43" s="143"/>
-      <c r="X43" s="143"/>
-      <c r="Y43" s="143"/>
-      <c r="Z43" s="143"/>
-      <c r="AA43" s="143"/>
-      <c r="AB43" s="143"/>
-      <c r="AC43" s="143"/>
+      <c r="C43" s="140"/>
+      <c r="D43" s="140"/>
+      <c r="E43" s="140"/>
+      <c r="F43" s="140"/>
+      <c r="G43" s="140"/>
+      <c r="H43" s="140"/>
+      <c r="I43" s="140"/>
+      <c r="J43" s="140"/>
+      <c r="K43" s="140"/>
+      <c r="L43" s="140"/>
+      <c r="M43" s="140"/>
+      <c r="N43" s="140"/>
+      <c r="O43" s="140"/>
+      <c r="P43" s="140"/>
+      <c r="Q43" s="140"/>
+      <c r="R43" s="140"/>
+      <c r="S43" s="140"/>
+      <c r="T43" s="140"/>
+      <c r="U43" s="140"/>
+      <c r="V43" s="140"/>
+      <c r="W43" s="140"/>
+      <c r="X43" s="140"/>
+      <c r="Y43" s="140"/>
+      <c r="Z43" s="140"/>
+      <c r="AA43" s="140"/>
+      <c r="AB43" s="140"/>
+      <c r="AC43" s="140"/>
       <c r="AE43" s="36"/>
       <c r="AG43" s="37"/>
       <c r="AJ43" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AL43" s="160"/>
-      <c r="AM43" s="160"/>
-      <c r="AN43" s="161"/>
+      <c r="AL43" s="157"/>
+      <c r="AM43" s="157"/>
+      <c r="AN43" s="158"/>
       <c r="AW43" s="38" t="s">
         <v>33</v>
       </c>
@@ -4518,45 +4514,45 @@
     <row r="45" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="94"/>
       <c r="B45" s="5"/>
-      <c r="C45" s="202"/>
-      <c r="D45" s="192"/>
-      <c r="E45" s="192"/>
-      <c r="F45" s="192"/>
-      <c r="G45" s="192"/>
-      <c r="H45" s="192"/>
-      <c r="I45" s="192"/>
-      <c r="J45" s="192"/>
-      <c r="K45" s="192"/>
-      <c r="L45" s="192"/>
-      <c r="M45" s="192"/>
-      <c r="N45" s="192"/>
-      <c r="O45" s="192"/>
-      <c r="P45" s="192"/>
-      <c r="Q45" s="192"/>
-      <c r="R45" s="192"/>
-      <c r="S45" s="192"/>
-      <c r="T45" s="192"/>
-      <c r="U45" s="192"/>
-      <c r="V45" s="192"/>
-      <c r="W45" s="192"/>
-      <c r="X45" s="192"/>
-      <c r="Y45" s="192"/>
-      <c r="Z45" s="192"/>
-      <c r="AA45" s="192"/>
-      <c r="AB45" s="192"/>
-      <c r="AC45" s="193"/>
+      <c r="C45" s="199"/>
+      <c r="D45" s="189"/>
+      <c r="E45" s="189"/>
+      <c r="F45" s="189"/>
+      <c r="G45" s="189"/>
+      <c r="H45" s="189"/>
+      <c r="I45" s="189"/>
+      <c r="J45" s="189"/>
+      <c r="K45" s="189"/>
+      <c r="L45" s="189"/>
+      <c r="M45" s="189"/>
+      <c r="N45" s="189"/>
+      <c r="O45" s="189"/>
+      <c r="P45" s="189"/>
+      <c r="Q45" s="189"/>
+      <c r="R45" s="189"/>
+      <c r="S45" s="189"/>
+      <c r="T45" s="189"/>
+      <c r="U45" s="189"/>
+      <c r="V45" s="189"/>
+      <c r="W45" s="189"/>
+      <c r="X45" s="189"/>
+      <c r="Y45" s="189"/>
+      <c r="Z45" s="189"/>
+      <c r="AA45" s="189"/>
+      <c r="AB45" s="189"/>
+      <c r="AC45" s="190"/>
       <c r="AD45" s="71"/>
       <c r="AE45" s="20"/>
       <c r="AG45" s="37"/>
       <c r="AJ45" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AL45" s="183">
+      <c r="AL45" s="180">
         <f>SUM(AL43+AL41)</f>
         <v>0</v>
       </c>
-      <c r="AM45" s="183"/>
-      <c r="AN45" s="184"/>
+      <c r="AM45" s="180"/>
+      <c r="AN45" s="181"/>
       <c r="AW45" s="38" t="s">
         <v>38</v>
       </c>
@@ -4564,33 +4560,33 @@
     <row r="46" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="94"/>
       <c r="B46" s="5"/>
-      <c r="C46" s="194"/>
-      <c r="D46" s="195"/>
-      <c r="E46" s="195"/>
-      <c r="F46" s="195"/>
-      <c r="G46" s="195"/>
-      <c r="H46" s="195"/>
-      <c r="I46" s="195"/>
-      <c r="J46" s="195"/>
-      <c r="K46" s="195"/>
-      <c r="L46" s="195"/>
-      <c r="M46" s="195"/>
-      <c r="N46" s="195"/>
-      <c r="O46" s="195"/>
-      <c r="P46" s="195"/>
-      <c r="Q46" s="195"/>
-      <c r="R46" s="195"/>
-      <c r="S46" s="195"/>
-      <c r="T46" s="195"/>
-      <c r="U46" s="195"/>
-      <c r="V46" s="195"/>
-      <c r="W46" s="195"/>
-      <c r="X46" s="195"/>
-      <c r="Y46" s="195"/>
-      <c r="Z46" s="195"/>
-      <c r="AA46" s="195"/>
-      <c r="AB46" s="195"/>
-      <c r="AC46" s="196"/>
+      <c r="C46" s="191"/>
+      <c r="D46" s="192"/>
+      <c r="E46" s="192"/>
+      <c r="F46" s="192"/>
+      <c r="G46" s="192"/>
+      <c r="H46" s="192"/>
+      <c r="I46" s="192"/>
+      <c r="J46" s="192"/>
+      <c r="K46" s="192"/>
+      <c r="L46" s="192"/>
+      <c r="M46" s="192"/>
+      <c r="N46" s="192"/>
+      <c r="O46" s="192"/>
+      <c r="P46" s="192"/>
+      <c r="Q46" s="192"/>
+      <c r="R46" s="192"/>
+      <c r="S46" s="192"/>
+      <c r="T46" s="192"/>
+      <c r="U46" s="192"/>
+      <c r="V46" s="192"/>
+      <c r="W46" s="192"/>
+      <c r="X46" s="192"/>
+      <c r="Y46" s="192"/>
+      <c r="Z46" s="192"/>
+      <c r="AA46" s="192"/>
+      <c r="AB46" s="192"/>
+      <c r="AC46" s="193"/>
       <c r="AD46" s="39"/>
       <c r="AE46" s="26"/>
       <c r="AG46" s="37"/>
@@ -4604,74 +4600,74 @@
     <row r="47" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="94"/>
       <c r="B47" s="5"/>
-      <c r="C47" s="194"/>
-      <c r="D47" s="195"/>
-      <c r="E47" s="195"/>
-      <c r="F47" s="195"/>
-      <c r="G47" s="195"/>
-      <c r="H47" s="195"/>
-      <c r="I47" s="195"/>
-      <c r="J47" s="195"/>
-      <c r="K47" s="195"/>
-      <c r="L47" s="195"/>
-      <c r="M47" s="195"/>
-      <c r="N47" s="195"/>
-      <c r="O47" s="195"/>
-      <c r="P47" s="195"/>
-      <c r="Q47" s="195"/>
-      <c r="R47" s="195"/>
-      <c r="S47" s="195"/>
-      <c r="T47" s="195"/>
-      <c r="U47" s="195"/>
-      <c r="V47" s="195"/>
-      <c r="W47" s="195"/>
-      <c r="X47" s="195"/>
-      <c r="Y47" s="195"/>
-      <c r="Z47" s="195"/>
-      <c r="AA47" s="195"/>
-      <c r="AB47" s="195"/>
-      <c r="AC47" s="196"/>
+      <c r="C47" s="191"/>
+      <c r="D47" s="192"/>
+      <c r="E47" s="192"/>
+      <c r="F47" s="192"/>
+      <c r="G47" s="192"/>
+      <c r="H47" s="192"/>
+      <c r="I47" s="192"/>
+      <c r="J47" s="192"/>
+      <c r="K47" s="192"/>
+      <c r="L47" s="192"/>
+      <c r="M47" s="192"/>
+      <c r="N47" s="192"/>
+      <c r="O47" s="192"/>
+      <c r="P47" s="192"/>
+      <c r="Q47" s="192"/>
+      <c r="R47" s="192"/>
+      <c r="S47" s="192"/>
+      <c r="T47" s="192"/>
+      <c r="U47" s="192"/>
+      <c r="V47" s="192"/>
+      <c r="W47" s="192"/>
+      <c r="X47" s="192"/>
+      <c r="Y47" s="192"/>
+      <c r="Z47" s="192"/>
+      <c r="AA47" s="192"/>
+      <c r="AB47" s="192"/>
+      <c r="AC47" s="193"/>
       <c r="AD47" s="39"/>
       <c r="AE47" s="26"/>
       <c r="AG47" s="37"/>
       <c r="AJ47" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AL47" s="187"/>
-      <c r="AM47" s="187"/>
-      <c r="AN47" s="188"/>
+      <c r="AL47" s="184"/>
+      <c r="AM47" s="184"/>
+      <c r="AN47" s="185"/>
       <c r="AW47" s="38"/>
     </row>
     <row r="48" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="94"/>
       <c r="B48" s="5"/>
-      <c r="C48" s="194"/>
-      <c r="D48" s="195"/>
-      <c r="E48" s="195"/>
-      <c r="F48" s="195"/>
-      <c r="G48" s="195"/>
-      <c r="H48" s="195"/>
-      <c r="I48" s="195"/>
-      <c r="J48" s="195"/>
-      <c r="K48" s="195"/>
-      <c r="L48" s="195"/>
-      <c r="M48" s="195"/>
-      <c r="N48" s="195"/>
-      <c r="O48" s="195"/>
-      <c r="P48" s="195"/>
-      <c r="Q48" s="195"/>
-      <c r="R48" s="195"/>
-      <c r="S48" s="195"/>
-      <c r="T48" s="195"/>
-      <c r="U48" s="195"/>
-      <c r="V48" s="195"/>
-      <c r="W48" s="195"/>
-      <c r="X48" s="195"/>
-      <c r="Y48" s="195"/>
-      <c r="Z48" s="195"/>
-      <c r="AA48" s="195"/>
-      <c r="AB48" s="195"/>
-      <c r="AC48" s="196"/>
+      <c r="C48" s="191"/>
+      <c r="D48" s="192"/>
+      <c r="E48" s="192"/>
+      <c r="F48" s="192"/>
+      <c r="G48" s="192"/>
+      <c r="H48" s="192"/>
+      <c r="I48" s="192"/>
+      <c r="J48" s="192"/>
+      <c r="K48" s="192"/>
+      <c r="L48" s="192"/>
+      <c r="M48" s="192"/>
+      <c r="N48" s="192"/>
+      <c r="O48" s="192"/>
+      <c r="P48" s="192"/>
+      <c r="Q48" s="192"/>
+      <c r="R48" s="192"/>
+      <c r="S48" s="192"/>
+      <c r="T48" s="192"/>
+      <c r="U48" s="192"/>
+      <c r="V48" s="192"/>
+      <c r="W48" s="192"/>
+      <c r="X48" s="192"/>
+      <c r="Y48" s="192"/>
+      <c r="Z48" s="192"/>
+      <c r="AA48" s="192"/>
+      <c r="AB48" s="192"/>
+      <c r="AC48" s="193"/>
       <c r="AD48" s="39"/>
       <c r="AE48" s="26"/>
       <c r="AG48" s="37"/>
@@ -4685,33 +4681,33 @@
     <row r="49" spans="1:49" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="94"/>
       <c r="B49" s="5"/>
-      <c r="C49" s="197"/>
-      <c r="D49" s="198"/>
-      <c r="E49" s="198"/>
-      <c r="F49" s="198"/>
-      <c r="G49" s="198"/>
-      <c r="H49" s="198"/>
-      <c r="I49" s="198"/>
-      <c r="J49" s="198"/>
-      <c r="K49" s="198"/>
-      <c r="L49" s="198"/>
-      <c r="M49" s="198"/>
-      <c r="N49" s="198"/>
-      <c r="O49" s="198"/>
-      <c r="P49" s="198"/>
-      <c r="Q49" s="198"/>
-      <c r="R49" s="198"/>
-      <c r="S49" s="198"/>
-      <c r="T49" s="198"/>
-      <c r="U49" s="198"/>
-      <c r="V49" s="198"/>
-      <c r="W49" s="198"/>
-      <c r="X49" s="198"/>
-      <c r="Y49" s="198"/>
-      <c r="Z49" s="198"/>
-      <c r="AA49" s="198"/>
-      <c r="AB49" s="198"/>
-      <c r="AC49" s="199"/>
+      <c r="C49" s="194"/>
+      <c r="D49" s="195"/>
+      <c r="E49" s="195"/>
+      <c r="F49" s="195"/>
+      <c r="G49" s="195"/>
+      <c r="H49" s="195"/>
+      <c r="I49" s="195"/>
+      <c r="J49" s="195"/>
+      <c r="K49" s="195"/>
+      <c r="L49" s="195"/>
+      <c r="M49" s="195"/>
+      <c r="N49" s="195"/>
+      <c r="O49" s="195"/>
+      <c r="P49" s="195"/>
+      <c r="Q49" s="195"/>
+      <c r="R49" s="195"/>
+      <c r="S49" s="195"/>
+      <c r="T49" s="195"/>
+      <c r="U49" s="195"/>
+      <c r="V49" s="195"/>
+      <c r="W49" s="195"/>
+      <c r="X49" s="195"/>
+      <c r="Y49" s="195"/>
+      <c r="Z49" s="195"/>
+      <c r="AA49" s="195"/>
+      <c r="AB49" s="195"/>
+      <c r="AC49" s="196"/>
       <c r="AD49" s="39"/>
       <c r="AE49" s="36"/>
       <c r="AG49" s="37"/>
@@ -4719,12 +4715,12 @@
         <v>37</v>
       </c>
       <c r="AK49" s="34"/>
-      <c r="AL49" s="183">
+      <c r="AL49" s="180">
         <f>SUM(AL47*AL45)</f>
         <v>0</v>
       </c>
-      <c r="AM49" s="183"/>
-      <c r="AN49" s="184"/>
+      <c r="AM49" s="180"/>
+      <c r="AN49" s="181"/>
       <c r="AW49" s="38" t="s">
         <v>40</v>
       </c>
@@ -4821,25 +4817,25 @@
       <c r="D52" s="126"/>
       <c r="E52" s="126"/>
       <c r="F52" s="126"/>
-      <c r="G52" s="153"/>
-      <c r="H52" s="154"/>
-      <c r="I52" s="154"/>
-      <c r="J52" s="154"/>
-      <c r="K52" s="154"/>
-      <c r="L52" s="154"/>
-      <c r="M52" s="154"/>
+      <c r="G52" s="150"/>
+      <c r="H52" s="151"/>
+      <c r="I52" s="151"/>
+      <c r="J52" s="151"/>
+      <c r="K52" s="151"/>
+      <c r="L52" s="151"/>
+      <c r="M52" s="151"/>
       <c r="O52" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="P52" s="141"/>
-      <c r="Q52" s="142"/>
-      <c r="R52" s="142"/>
-      <c r="S52" s="142"/>
+      <c r="P52" s="138"/>
+      <c r="Q52" s="139"/>
+      <c r="R52" s="139"/>
+      <c r="S52" s="139"/>
       <c r="T52" s="56"/>
-      <c r="U52" s="135" t="s">
+      <c r="U52" s="132" t="s">
         <v>24</v>
       </c>
-      <c r="V52" s="144"/>
+      <c r="V52" s="141"/>
       <c r="W52" s="127"/>
       <c r="X52" s="127"/>
       <c r="Y52" s="127"/>
@@ -4855,7 +4851,7 @@
       <c r="AW52" s="6"/>
     </row>
     <row r="53" spans="1:49" ht="5.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="148" t="s">
+      <c r="A53" s="145" t="s">
         <v>26</v>
       </c>
       <c r="B53" s="5"/>
@@ -4864,7 +4860,7 @@
       <c r="AW53" s="6"/>
     </row>
     <row r="54" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="148"/>
+      <c r="A54" s="145"/>
       <c r="B54" s="5"/>
       <c r="C54" s="57" t="s">
         <v>45</v>
@@ -4898,9 +4894,9 @@
       <c r="AJ54" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AL54" s="160"/>
-      <c r="AM54" s="160"/>
-      <c r="AN54" s="161"/>
+      <c r="AL54" s="157"/>
+      <c r="AM54" s="157"/>
+      <c r="AN54" s="158"/>
       <c r="AW54" s="6"/>
     </row>
     <row r="55" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4908,33 +4904,33 @@
         <v>30</v>
       </c>
       <c r="B55" s="5"/>
-      <c r="C55" s="140"/>
-      <c r="D55" s="140"/>
-      <c r="E55" s="140"/>
-      <c r="F55" s="140"/>
-      <c r="G55" s="140"/>
-      <c r="H55" s="140"/>
-      <c r="I55" s="140"/>
-      <c r="J55" s="140"/>
-      <c r="K55" s="140"/>
+      <c r="C55" s="137"/>
+      <c r="D55" s="137"/>
+      <c r="E55" s="137"/>
+      <c r="F55" s="137"/>
+      <c r="G55" s="137"/>
+      <c r="H55" s="137"/>
+      <c r="I55" s="137"/>
+      <c r="J55" s="137"/>
+      <c r="K55" s="137"/>
       <c r="L55" s="24"/>
-      <c r="M55" s="149"/>
-      <c r="N55" s="149"/>
-      <c r="O55" s="149"/>
-      <c r="P55" s="149"/>
-      <c r="Q55" s="149"/>
-      <c r="R55" s="149"/>
-      <c r="S55" s="149"/>
-      <c r="T55" s="149"/>
-      <c r="U55" s="149"/>
-      <c r="V55" s="149"/>
-      <c r="W55" s="149"/>
-      <c r="X55" s="149"/>
-      <c r="Y55" s="149"/>
-      <c r="Z55" s="149"/>
-      <c r="AA55" s="149"/>
-      <c r="AB55" s="149"/>
-      <c r="AC55" s="149"/>
+      <c r="M55" s="146"/>
+      <c r="N55" s="146"/>
+      <c r="O55" s="146"/>
+      <c r="P55" s="146"/>
+      <c r="Q55" s="146"/>
+      <c r="R55" s="146"/>
+      <c r="S55" s="146"/>
+      <c r="T55" s="146"/>
+      <c r="U55" s="146"/>
+      <c r="V55" s="146"/>
+      <c r="W55" s="146"/>
+      <c r="X55" s="146"/>
+      <c r="Y55" s="146"/>
+      <c r="Z55" s="146"/>
+      <c r="AA55" s="146"/>
+      <c r="AB55" s="146"/>
+      <c r="AC55" s="146"/>
       <c r="AG55" s="37"/>
       <c r="AN55" s="18"/>
       <c r="AW55" s="38" t="s">
@@ -4944,10 +4940,10 @@
     <row r="56" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="97"/>
       <c r="B56" s="5"/>
-      <c r="C56" s="190"/>
-      <c r="D56" s="190"/>
-      <c r="E56" s="190"/>
-      <c r="F56" s="190"/>
+      <c r="C56" s="187"/>
+      <c r="D56" s="187"/>
+      <c r="E56" s="187"/>
+      <c r="F56" s="187"/>
       <c r="G56" s="39"/>
       <c r="H56" s="39"/>
       <c r="AE56" s="36"/>
@@ -4955,9 +4951,9 @@
       <c r="AJ56" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AL56" s="160"/>
-      <c r="AM56" s="160"/>
-      <c r="AN56" s="161"/>
+      <c r="AL56" s="157"/>
+      <c r="AM56" s="157"/>
+      <c r="AN56" s="158"/>
       <c r="AW56" s="38" t="s">
         <v>33</v>
       </c>
@@ -5007,45 +5003,45 @@
     <row r="58" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="94"/>
       <c r="B58" s="5"/>
-      <c r="C58" s="191"/>
-      <c r="D58" s="192"/>
-      <c r="E58" s="192"/>
-      <c r="F58" s="192"/>
-      <c r="G58" s="192"/>
-      <c r="H58" s="192"/>
-      <c r="I58" s="192"/>
-      <c r="J58" s="192"/>
-      <c r="K58" s="192"/>
-      <c r="L58" s="192"/>
-      <c r="M58" s="192"/>
-      <c r="N58" s="192"/>
-      <c r="O58" s="192"/>
-      <c r="P58" s="192"/>
-      <c r="Q58" s="192"/>
-      <c r="R58" s="192"/>
-      <c r="S58" s="192"/>
-      <c r="T58" s="192"/>
-      <c r="U58" s="192"/>
-      <c r="V58" s="192"/>
-      <c r="W58" s="192"/>
-      <c r="X58" s="192"/>
-      <c r="Y58" s="192"/>
-      <c r="Z58" s="192"/>
-      <c r="AA58" s="192"/>
-      <c r="AB58" s="192"/>
-      <c r="AC58" s="193"/>
+      <c r="C58" s="188"/>
+      <c r="D58" s="189"/>
+      <c r="E58" s="189"/>
+      <c r="F58" s="189"/>
+      <c r="G58" s="189"/>
+      <c r="H58" s="189"/>
+      <c r="I58" s="189"/>
+      <c r="J58" s="189"/>
+      <c r="K58" s="189"/>
+      <c r="L58" s="189"/>
+      <c r="M58" s="189"/>
+      <c r="N58" s="189"/>
+      <c r="O58" s="189"/>
+      <c r="P58" s="189"/>
+      <c r="Q58" s="189"/>
+      <c r="R58" s="189"/>
+      <c r="S58" s="189"/>
+      <c r="T58" s="189"/>
+      <c r="U58" s="189"/>
+      <c r="V58" s="189"/>
+      <c r="W58" s="189"/>
+      <c r="X58" s="189"/>
+      <c r="Y58" s="189"/>
+      <c r="Z58" s="189"/>
+      <c r="AA58" s="189"/>
+      <c r="AB58" s="189"/>
+      <c r="AC58" s="190"/>
       <c r="AD58" s="40"/>
       <c r="AE58" s="20"/>
       <c r="AG58" s="37"/>
       <c r="AJ58" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AL58" s="183">
+      <c r="AL58" s="180">
         <f>SUM(AL56+AL54)</f>
         <v>0</v>
       </c>
-      <c r="AM58" s="183"/>
-      <c r="AN58" s="184"/>
+      <c r="AM58" s="180"/>
+      <c r="AN58" s="181"/>
       <c r="AW58" s="38" t="s">
         <v>38</v>
       </c>
@@ -5053,33 +5049,33 @@
     <row r="59" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="94"/>
       <c r="B59" s="5"/>
-      <c r="C59" s="194"/>
-      <c r="D59" s="195"/>
-      <c r="E59" s="195"/>
-      <c r="F59" s="195"/>
-      <c r="G59" s="195"/>
-      <c r="H59" s="195"/>
-      <c r="I59" s="195"/>
-      <c r="J59" s="195"/>
-      <c r="K59" s="195"/>
-      <c r="L59" s="195"/>
-      <c r="M59" s="195"/>
-      <c r="N59" s="195"/>
-      <c r="O59" s="195"/>
-      <c r="P59" s="195"/>
-      <c r="Q59" s="195"/>
-      <c r="R59" s="195"/>
-      <c r="S59" s="195"/>
-      <c r="T59" s="195"/>
-      <c r="U59" s="195"/>
-      <c r="V59" s="195"/>
-      <c r="W59" s="195"/>
-      <c r="X59" s="195"/>
-      <c r="Y59" s="195"/>
-      <c r="Z59" s="195"/>
-      <c r="AA59" s="195"/>
-      <c r="AB59" s="195"/>
-      <c r="AC59" s="196"/>
+      <c r="C59" s="191"/>
+      <c r="D59" s="192"/>
+      <c r="E59" s="192"/>
+      <c r="F59" s="192"/>
+      <c r="G59" s="192"/>
+      <c r="H59" s="192"/>
+      <c r="I59" s="192"/>
+      <c r="J59" s="192"/>
+      <c r="K59" s="192"/>
+      <c r="L59" s="192"/>
+      <c r="M59" s="192"/>
+      <c r="N59" s="192"/>
+      <c r="O59" s="192"/>
+      <c r="P59" s="192"/>
+      <c r="Q59" s="192"/>
+      <c r="R59" s="192"/>
+      <c r="S59" s="192"/>
+      <c r="T59" s="192"/>
+      <c r="U59" s="192"/>
+      <c r="V59" s="192"/>
+      <c r="W59" s="192"/>
+      <c r="X59" s="192"/>
+      <c r="Y59" s="192"/>
+      <c r="Z59" s="192"/>
+      <c r="AA59" s="192"/>
+      <c r="AB59" s="192"/>
+      <c r="AC59" s="193"/>
       <c r="AD59" s="39"/>
       <c r="AE59" s="26"/>
       <c r="AG59" s="37"/>
@@ -5093,74 +5089,74 @@
     <row r="60" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="94"/>
       <c r="B60" s="5"/>
-      <c r="C60" s="194"/>
-      <c r="D60" s="195"/>
-      <c r="E60" s="195"/>
-      <c r="F60" s="195"/>
-      <c r="G60" s="195"/>
-      <c r="H60" s="195"/>
-      <c r="I60" s="195"/>
-      <c r="J60" s="195"/>
-      <c r="K60" s="195"/>
-      <c r="L60" s="195"/>
-      <c r="M60" s="195"/>
-      <c r="N60" s="195"/>
-      <c r="O60" s="195"/>
-      <c r="P60" s="195"/>
-      <c r="Q60" s="195"/>
-      <c r="R60" s="195"/>
-      <c r="S60" s="195"/>
-      <c r="T60" s="195"/>
-      <c r="U60" s="195"/>
-      <c r="V60" s="195"/>
-      <c r="W60" s="195"/>
-      <c r="X60" s="195"/>
-      <c r="Y60" s="195"/>
-      <c r="Z60" s="195"/>
-      <c r="AA60" s="195"/>
-      <c r="AB60" s="195"/>
-      <c r="AC60" s="196"/>
+      <c r="C60" s="191"/>
+      <c r="D60" s="192"/>
+      <c r="E60" s="192"/>
+      <c r="F60" s="192"/>
+      <c r="G60" s="192"/>
+      <c r="H60" s="192"/>
+      <c r="I60" s="192"/>
+      <c r="J60" s="192"/>
+      <c r="K60" s="192"/>
+      <c r="L60" s="192"/>
+      <c r="M60" s="192"/>
+      <c r="N60" s="192"/>
+      <c r="O60" s="192"/>
+      <c r="P60" s="192"/>
+      <c r="Q60" s="192"/>
+      <c r="R60" s="192"/>
+      <c r="S60" s="192"/>
+      <c r="T60" s="192"/>
+      <c r="U60" s="192"/>
+      <c r="V60" s="192"/>
+      <c r="W60" s="192"/>
+      <c r="X60" s="192"/>
+      <c r="Y60" s="192"/>
+      <c r="Z60" s="192"/>
+      <c r="AA60" s="192"/>
+      <c r="AB60" s="192"/>
+      <c r="AC60" s="193"/>
       <c r="AD60" s="39"/>
       <c r="AE60" s="26"/>
       <c r="AG60" s="37"/>
       <c r="AJ60" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AL60" s="187"/>
-      <c r="AM60" s="187"/>
-      <c r="AN60" s="188"/>
+      <c r="AL60" s="184"/>
+      <c r="AM60" s="184"/>
+      <c r="AN60" s="185"/>
       <c r="AW60" s="38"/>
     </row>
     <row r="61" spans="1:49" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="94"/>
       <c r="B61" s="5"/>
-      <c r="C61" s="194"/>
-      <c r="D61" s="195"/>
-      <c r="E61" s="195"/>
-      <c r="F61" s="195"/>
-      <c r="G61" s="195"/>
-      <c r="H61" s="195"/>
-      <c r="I61" s="195"/>
-      <c r="J61" s="195"/>
-      <c r="K61" s="195"/>
-      <c r="L61" s="195"/>
-      <c r="M61" s="195"/>
-      <c r="N61" s="195"/>
-      <c r="O61" s="195"/>
-      <c r="P61" s="195"/>
-      <c r="Q61" s="195"/>
-      <c r="R61" s="195"/>
-      <c r="S61" s="195"/>
-      <c r="T61" s="195"/>
-      <c r="U61" s="195"/>
-      <c r="V61" s="195"/>
-      <c r="W61" s="195"/>
-      <c r="X61" s="195"/>
-      <c r="Y61" s="195"/>
-      <c r="Z61" s="195"/>
-      <c r="AA61" s="195"/>
-      <c r="AB61" s="195"/>
-      <c r="AC61" s="196"/>
+      <c r="C61" s="191"/>
+      <c r="D61" s="192"/>
+      <c r="E61" s="192"/>
+      <c r="F61" s="192"/>
+      <c r="G61" s="192"/>
+      <c r="H61" s="192"/>
+      <c r="I61" s="192"/>
+      <c r="J61" s="192"/>
+      <c r="K61" s="192"/>
+      <c r="L61" s="192"/>
+      <c r="M61" s="192"/>
+      <c r="N61" s="192"/>
+      <c r="O61" s="192"/>
+      <c r="P61" s="192"/>
+      <c r="Q61" s="192"/>
+      <c r="R61" s="192"/>
+      <c r="S61" s="192"/>
+      <c r="T61" s="192"/>
+      <c r="U61" s="192"/>
+      <c r="V61" s="192"/>
+      <c r="W61" s="192"/>
+      <c r="X61" s="192"/>
+      <c r="Y61" s="192"/>
+      <c r="Z61" s="192"/>
+      <c r="AA61" s="192"/>
+      <c r="AB61" s="192"/>
+      <c r="AC61" s="193"/>
       <c r="AD61" s="39"/>
       <c r="AE61" s="26"/>
       <c r="AG61" s="37"/>
@@ -5174,33 +5170,33 @@
     <row r="62" spans="1:49" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="94"/>
       <c r="B62" s="5"/>
-      <c r="C62" s="197"/>
-      <c r="D62" s="198"/>
-      <c r="E62" s="198"/>
-      <c r="F62" s="198"/>
-      <c r="G62" s="198"/>
-      <c r="H62" s="198"/>
-      <c r="I62" s="198"/>
-      <c r="J62" s="198"/>
-      <c r="K62" s="198"/>
-      <c r="L62" s="198"/>
-      <c r="M62" s="198"/>
-      <c r="N62" s="198"/>
-      <c r="O62" s="198"/>
-      <c r="P62" s="198"/>
-      <c r="Q62" s="198"/>
-      <c r="R62" s="198"/>
-      <c r="S62" s="198"/>
-      <c r="T62" s="198"/>
-      <c r="U62" s="198"/>
-      <c r="V62" s="198"/>
-      <c r="W62" s="198"/>
-      <c r="X62" s="198"/>
-      <c r="Y62" s="198"/>
-      <c r="Z62" s="198"/>
-      <c r="AA62" s="198"/>
-      <c r="AB62" s="198"/>
-      <c r="AC62" s="199"/>
+      <c r="C62" s="194"/>
+      <c r="D62" s="195"/>
+      <c r="E62" s="195"/>
+      <c r="F62" s="195"/>
+      <c r="G62" s="195"/>
+      <c r="H62" s="195"/>
+      <c r="I62" s="195"/>
+      <c r="J62" s="195"/>
+      <c r="K62" s="195"/>
+      <c r="L62" s="195"/>
+      <c r="M62" s="195"/>
+      <c r="N62" s="195"/>
+      <c r="O62" s="195"/>
+      <c r="P62" s="195"/>
+      <c r="Q62" s="195"/>
+      <c r="R62" s="195"/>
+      <c r="S62" s="195"/>
+      <c r="T62" s="195"/>
+      <c r="U62" s="195"/>
+      <c r="V62" s="195"/>
+      <c r="W62" s="195"/>
+      <c r="X62" s="195"/>
+      <c r="Y62" s="195"/>
+      <c r="Z62" s="195"/>
+      <c r="AA62" s="195"/>
+      <c r="AB62" s="195"/>
+      <c r="AC62" s="196"/>
       <c r="AD62" s="39"/>
       <c r="AE62" s="36"/>
       <c r="AG62" s="37"/>
@@ -5208,12 +5204,12 @@
         <v>37</v>
       </c>
       <c r="AK62" s="34"/>
-      <c r="AL62" s="183">
+      <c r="AL62" s="180">
         <f>SUM(AL60*AL58)</f>
         <v>0</v>
       </c>
-      <c r="AM62" s="183"/>
-      <c r="AN62" s="184"/>
+      <c r="AM62" s="180"/>
+      <c r="AN62" s="181"/>
       <c r="AW62" s="38" t="s">
         <v>40</v>
       </c>
@@ -5276,33 +5272,33 @@
         <v>46</v>
       </c>
       <c r="B65" s="5"/>
-      <c r="C65" s="189" t="s">
+      <c r="C65" s="186" t="s">
         <v>47</v>
       </c>
-      <c r="D65" s="189"/>
-      <c r="E65" s="189"/>
-      <c r="F65" s="189"/>
-      <c r="G65" s="189"/>
-      <c r="H65" s="189"/>
-      <c r="I65" s="189"/>
-      <c r="J65" s="189"/>
-      <c r="K65" s="189"/>
+      <c r="D65" s="186"/>
+      <c r="E65" s="186"/>
+      <c r="F65" s="186"/>
+      <c r="G65" s="186"/>
+      <c r="H65" s="186"/>
+      <c r="I65" s="186"/>
+      <c r="J65" s="186"/>
+      <c r="K65" s="186"/>
       <c r="L65" s="36"/>
-      <c r="T65" s="162" t="s">
+      <c r="T65" s="159" t="s">
         <v>48</v>
       </c>
-      <c r="U65" s="163"/>
-      <c r="V65" s="163"/>
-      <c r="W65" s="163"/>
-      <c r="X65" s="163"/>
-      <c r="Y65" s="163"/>
-      <c r="Z65" s="163"/>
-      <c r="AA65" s="163"/>
-      <c r="AB65" s="163"/>
-      <c r="AC65" s="163"/>
-      <c r="AD65" s="163"/>
-      <c r="AE65" s="163"/>
-      <c r="AF65" s="163"/>
+      <c r="U65" s="160"/>
+      <c r="V65" s="160"/>
+      <c r="W65" s="160"/>
+      <c r="X65" s="160"/>
+      <c r="Y65" s="160"/>
+      <c r="Z65" s="160"/>
+      <c r="AA65" s="160"/>
+      <c r="AB65" s="160"/>
+      <c r="AC65" s="160"/>
+      <c r="AD65" s="160"/>
+      <c r="AE65" s="160"/>
+      <c r="AF65" s="160"/>
       <c r="AG65" s="37"/>
       <c r="AH65" s="34" t="s">
         <v>25</v>
@@ -5327,34 +5323,34 @@
     <row r="67" spans="1:48" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="94"/>
       <c r="B67" s="5"/>
-      <c r="U67" s="155" t="s">
+      <c r="U67" s="152" t="s">
         <v>49</v>
       </c>
-      <c r="V67" s="155"/>
-      <c r="W67" s="155"/>
-      <c r="X67" s="139" t="s">
+      <c r="V67" s="152"/>
+      <c r="W67" s="152"/>
+      <c r="X67" s="136" t="s">
         <v>50</v>
       </c>
-      <c r="Y67" s="139"/>
-      <c r="Z67" s="139"/>
-      <c r="AA67" s="139" t="s">
+      <c r="Y67" s="136"/>
+      <c r="Z67" s="136"/>
+      <c r="AA67" s="136" t="s">
         <v>51</v>
       </c>
-      <c r="AB67" s="139"/>
-      <c r="AC67" s="139"/>
+      <c r="AB67" s="136"/>
+      <c r="AC67" s="136"/>
       <c r="AD67" s="24"/>
       <c r="AG67" s="37"/>
-      <c r="AH67" s="137" t="s">
+      <c r="AH67" s="134" t="s">
         <v>52</v>
       </c>
-      <c r="AI67" s="138"/>
-      <c r="AJ67" s="138"/>
-      <c r="AK67" s="138"/>
-      <c r="AL67" s="185" t="s">
+      <c r="AI67" s="135"/>
+      <c r="AJ67" s="135"/>
+      <c r="AK67" s="135"/>
+      <c r="AL67" s="182" t="s">
         <v>53</v>
       </c>
-      <c r="AM67" s="185"/>
-      <c r="AN67" s="186"/>
+      <c r="AM67" s="182"/>
+      <c r="AN67" s="183"/>
       <c r="AV67" s="6"/>
     </row>
     <row r="68" spans="1:48" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5383,10 +5379,10 @@
       <c r="U68" s="112"/>
       <c r="V68" s="54"/>
       <c r="Y68" s="54"/>
-      <c r="AB68" s="200">
+      <c r="AB68" s="197">
         <v>0.8</v>
       </c>
-      <c r="AC68" s="201"/>
+      <c r="AC68" s="198"/>
       <c r="AG68" s="37"/>
       <c r="AN68" s="18"/>
       <c r="AV68" s="6"/>
@@ -5395,66 +5391,66 @@
       <c r="A69" s="94"/>
       <c r="B69" s="5"/>
       <c r="C69" s="112"/>
-      <c r="D69" s="215" t="s">
+      <c r="D69" s="212" t="s">
         <v>55</v>
       </c>
-      <c r="E69" s="215"/>
-      <c r="F69" s="215"/>
-      <c r="G69" s="215"/>
-      <c r="H69" s="215"/>
-      <c r="I69" s="215"/>
-      <c r="J69" s="215"/>
-      <c r="K69" s="215"/>
-      <c r="L69" s="215"/>
-      <c r="M69" s="215"/>
-      <c r="N69" s="215"/>
-      <c r="O69" s="215"/>
-      <c r="P69" s="215"/>
-      <c r="Q69" s="215"/>
-      <c r="R69" s="215"/>
-      <c r="S69" s="215"/>
-      <c r="T69" s="215"/>
-      <c r="U69" s="215"/>
+      <c r="E69" s="212"/>
+      <c r="F69" s="212"/>
+      <c r="G69" s="212"/>
+      <c r="H69" s="212"/>
+      <c r="I69" s="212"/>
+      <c r="J69" s="212"/>
+      <c r="K69" s="212"/>
+      <c r="L69" s="212"/>
+      <c r="M69" s="212"/>
+      <c r="N69" s="212"/>
+      <c r="O69" s="212"/>
+      <c r="P69" s="212"/>
+      <c r="Q69" s="212"/>
+      <c r="R69" s="212"/>
+      <c r="S69" s="212"/>
+      <c r="T69" s="212"/>
+      <c r="U69" s="212"/>
       <c r="V69" s="45"/>
       <c r="W69" s="45"/>
       <c r="Y69" s="8"/>
       <c r="AG69" s="37"/>
-      <c r="AH69" s="137" t="s">
+      <c r="AH69" s="134" t="s">
         <v>56</v>
       </c>
-      <c r="AI69" s="138"/>
-      <c r="AJ69" s="138"/>
-      <c r="AK69" s="138"/>
-      <c r="AL69" s="183">
+      <c r="AI69" s="135"/>
+      <c r="AJ69" s="135"/>
+      <c r="AK69" s="135"/>
+      <c r="AL69" s="180">
         <f>+AL62+AL49+AL36</f>
         <v>0</v>
       </c>
-      <c r="AM69" s="183"/>
-      <c r="AN69" s="184"/>
+      <c r="AM69" s="180"/>
+      <c r="AN69" s="181"/>
       <c r="AV69" s="6"/>
     </row>
     <row r="70" spans="1:48" ht="13.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="94"/>
       <c r="B70" s="5"/>
       <c r="C70" s="112"/>
-      <c r="D70" s="215"/>
-      <c r="E70" s="215"/>
-      <c r="F70" s="215"/>
-      <c r="G70" s="215"/>
-      <c r="H70" s="215"/>
-      <c r="I70" s="215"/>
-      <c r="J70" s="215"/>
-      <c r="K70" s="215"/>
-      <c r="L70" s="215"/>
-      <c r="M70" s="215"/>
-      <c r="N70" s="215"/>
-      <c r="O70" s="215"/>
-      <c r="P70" s="215"/>
-      <c r="Q70" s="215"/>
-      <c r="R70" s="215"/>
-      <c r="S70" s="215"/>
-      <c r="T70" s="215"/>
-      <c r="U70" s="215"/>
+      <c r="D70" s="212"/>
+      <c r="E70" s="212"/>
+      <c r="F70" s="212"/>
+      <c r="G70" s="212"/>
+      <c r="H70" s="212"/>
+      <c r="I70" s="212"/>
+      <c r="J70" s="212"/>
+      <c r="K70" s="212"/>
+      <c r="L70" s="212"/>
+      <c r="M70" s="212"/>
+      <c r="N70" s="212"/>
+      <c r="O70" s="212"/>
+      <c r="P70" s="212"/>
+      <c r="Q70" s="212"/>
+      <c r="R70" s="212"/>
+      <c r="S70" s="212"/>
+      <c r="T70" s="212"/>
+      <c r="U70" s="212"/>
       <c r="V70" s="45"/>
       <c r="W70" s="45"/>
       <c r="Y70" s="30"/>
@@ -5468,76 +5464,76 @@
     <row r="71" spans="1:48" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="94"/>
       <c r="B71" s="5"/>
-      <c r="C71" s="156" t="s">
+      <c r="C71" s="153" t="s">
         <v>57</v>
       </c>
-      <c r="D71" s="156"/>
-      <c r="E71" s="156"/>
-      <c r="F71" s="156"/>
-      <c r="G71" s="156"/>
-      <c r="H71" s="156"/>
-      <c r="I71" s="156"/>
-      <c r="J71" s="156"/>
-      <c r="K71" s="156"/>
-      <c r="L71" s="156"/>
-      <c r="M71" s="156"/>
-      <c r="N71" s="156"/>
-      <c r="O71" s="156"/>
-      <c r="P71" s="156"/>
-      <c r="Q71" s="156"/>
-      <c r="R71" s="156"/>
-      <c r="S71" s="156"/>
-      <c r="T71" s="156"/>
-      <c r="U71" s="157"/>
+      <c r="D71" s="153"/>
+      <c r="E71" s="153"/>
+      <c r="F71" s="153"/>
+      <c r="G71" s="153"/>
+      <c r="H71" s="153"/>
+      <c r="I71" s="153"/>
+      <c r="J71" s="153"/>
+      <c r="K71" s="153"/>
+      <c r="L71" s="153"/>
+      <c r="M71" s="153"/>
+      <c r="N71" s="153"/>
+      <c r="O71" s="153"/>
+      <c r="P71" s="153"/>
+      <c r="Q71" s="153"/>
+      <c r="R71" s="153"/>
+      <c r="S71" s="153"/>
+      <c r="T71" s="153"/>
+      <c r="U71" s="154"/>
       <c r="V71" s="54"/>
       <c r="Y71" s="54"/>
-      <c r="AB71" s="137"/>
-      <c r="AC71" s="144"/>
+      <c r="AB71" s="134"/>
+      <c r="AC71" s="141"/>
       <c r="AD71" s="36"/>
       <c r="AG71" s="37"/>
-      <c r="AH71" s="137" t="s">
+      <c r="AH71" s="134" t="s">
         <v>58</v>
       </c>
-      <c r="AI71" s="137"/>
-      <c r="AJ71" s="137"/>
-      <c r="AK71" s="138"/>
-      <c r="AL71" s="160">
+      <c r="AI71" s="134"/>
+      <c r="AJ71" s="134"/>
+      <c r="AK71" s="135"/>
+      <c r="AL71" s="157">
         <v>1000000</v>
       </c>
-      <c r="AM71" s="160"/>
-      <c r="AN71" s="161"/>
+      <c r="AM71" s="157"/>
+      <c r="AN71" s="158"/>
       <c r="AV71" s="6"/>
     </row>
     <row r="72" spans="1:48" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="94"/>
       <c r="B72" s="5"/>
-      <c r="C72" s="156" t="s">
+      <c r="C72" s="153" t="s">
         <v>59</v>
       </c>
-      <c r="D72" s="156"/>
-      <c r="E72" s="156"/>
-      <c r="F72" s="156"/>
-      <c r="G72" s="156"/>
-      <c r="H72" s="156"/>
-      <c r="I72" s="156"/>
-      <c r="J72" s="156"/>
-      <c r="K72" s="156"/>
-      <c r="L72" s="156"/>
-      <c r="M72" s="156"/>
-      <c r="N72" s="156"/>
-      <c r="O72" s="156"/>
-      <c r="P72" s="156"/>
-      <c r="Q72" s="156"/>
-      <c r="R72" s="156"/>
-      <c r="S72" s="156"/>
-      <c r="T72" s="156"/>
-      <c r="U72" s="157"/>
+      <c r="D72" s="153"/>
+      <c r="E72" s="153"/>
+      <c r="F72" s="153"/>
+      <c r="G72" s="153"/>
+      <c r="H72" s="153"/>
+      <c r="I72" s="153"/>
+      <c r="J72" s="153"/>
+      <c r="K72" s="153"/>
+      <c r="L72" s="153"/>
+      <c r="M72" s="153"/>
+      <c r="N72" s="153"/>
+      <c r="O72" s="153"/>
+      <c r="P72" s="153"/>
+      <c r="Q72" s="153"/>
+      <c r="R72" s="153"/>
+      <c r="S72" s="153"/>
+      <c r="T72" s="153"/>
+      <c r="U72" s="154"/>
       <c r="V72" s="54"/>
       <c r="X72" s="47"/>
       <c r="Y72" s="54"/>
       <c r="Z72" s="55"/>
-      <c r="AB72" s="137"/>
-      <c r="AC72" s="144"/>
+      <c r="AB72" s="134"/>
+      <c r="AC72" s="141"/>
       <c r="AG72" s="37"/>
       <c r="AL72" s="79"/>
       <c r="AM72" s="79"/>
@@ -5547,42 +5543,42 @@
     <row r="73" spans="1:48" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="94"/>
       <c r="B73" s="5"/>
-      <c r="C73" s="156" t="s">
+      <c r="C73" s="153" t="s">
         <v>60</v>
       </c>
-      <c r="D73" s="156"/>
-      <c r="E73" s="156"/>
-      <c r="F73" s="156"/>
-      <c r="G73" s="156"/>
-      <c r="H73" s="156"/>
-      <c r="I73" s="156"/>
-      <c r="J73" s="156"/>
-      <c r="K73" s="156"/>
-      <c r="L73" s="156"/>
-      <c r="M73" s="156"/>
-      <c r="N73" s="156"/>
-      <c r="O73" s="156"/>
-      <c r="P73" s="156"/>
-      <c r="Q73" s="156"/>
-      <c r="R73" s="156"/>
-      <c r="S73" s="156"/>
-      <c r="T73" s="156"/>
-      <c r="U73" s="157"/>
+      <c r="D73" s="153"/>
+      <c r="E73" s="153"/>
+      <c r="F73" s="153"/>
+      <c r="G73" s="153"/>
+      <c r="H73" s="153"/>
+      <c r="I73" s="153"/>
+      <c r="J73" s="153"/>
+      <c r="K73" s="153"/>
+      <c r="L73" s="153"/>
+      <c r="M73" s="153"/>
+      <c r="N73" s="153"/>
+      <c r="O73" s="153"/>
+      <c r="P73" s="153"/>
+      <c r="Q73" s="153"/>
+      <c r="R73" s="153"/>
+      <c r="S73" s="153"/>
+      <c r="T73" s="153"/>
+      <c r="U73" s="154"/>
       <c r="V73" s="54"/>
       <c r="X73" s="52"/>
       <c r="Y73" s="54"/>
-      <c r="AB73" s="137"/>
-      <c r="AC73" s="144"/>
+      <c r="AB73" s="134"/>
+      <c r="AC73" s="141"/>
       <c r="AG73" s="37"/>
-      <c r="AH73" s="137" t="s">
+      <c r="AH73" s="134" t="s">
         <v>61</v>
       </c>
-      <c r="AI73" s="137"/>
-      <c r="AJ73" s="137"/>
-      <c r="AK73" s="138"/>
-      <c r="AL73" s="160"/>
-      <c r="AM73" s="160"/>
-      <c r="AN73" s="161"/>
+      <c r="AI73" s="134"/>
+      <c r="AJ73" s="134"/>
+      <c r="AK73" s="135"/>
+      <c r="AL73" s="157"/>
+      <c r="AM73" s="157"/>
+      <c r="AN73" s="158"/>
       <c r="AV73" s="6"/>
     </row>
     <row r="74" spans="1:48" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5623,35 +5619,35 @@
     <row r="75" spans="1:48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="94"/>
       <c r="B75" s="5"/>
-      <c r="C75" s="213" t="s">
+      <c r="C75" s="210" t="s">
         <v>63</v>
       </c>
-      <c r="D75" s="214"/>
-      <c r="E75" s="214"/>
-      <c r="F75" s="214"/>
-      <c r="G75" s="214"/>
-      <c r="H75" s="214"/>
-      <c r="I75" s="214"/>
-      <c r="J75" s="214"/>
-      <c r="K75" s="214"/>
-      <c r="L75" s="214"/>
-      <c r="M75" s="214"/>
-      <c r="N75" s="214"/>
-      <c r="O75" s="214"/>
-      <c r="P75" s="214"/>
-      <c r="Q75" s="214"/>
-      <c r="R75" s="214"/>
-      <c r="S75" s="214"/>
-      <c r="T75" s="214"/>
-      <c r="U75" s="214"/>
+      <c r="D75" s="211"/>
+      <c r="E75" s="211"/>
+      <c r="F75" s="211"/>
+      <c r="G75" s="211"/>
+      <c r="H75" s="211"/>
+      <c r="I75" s="211"/>
+      <c r="J75" s="211"/>
+      <c r="K75" s="211"/>
+      <c r="L75" s="211"/>
+      <c r="M75" s="211"/>
+      <c r="N75" s="211"/>
+      <c r="O75" s="211"/>
+      <c r="P75" s="211"/>
+      <c r="Q75" s="211"/>
+      <c r="R75" s="211"/>
+      <c r="S75" s="211"/>
+      <c r="T75" s="211"/>
+      <c r="U75" s="211"/>
       <c r="V75" s="65"/>
       <c r="W75" s="8"/>
       <c r="X75" s="66"/>
       <c r="Y75" s="65"/>
       <c r="Z75" s="8"/>
       <c r="AA75" s="8"/>
-      <c r="AB75" s="158"/>
-      <c r="AC75" s="159"/>
+      <c r="AB75" s="155"/>
+      <c r="AC75" s="156"/>
       <c r="AG75" s="37"/>
       <c r="AL75" s="79"/>
       <c r="AM75" s="79"/>
@@ -5685,10 +5681,7 @@
       <c r="Y76" s="58"/>
       <c r="AC76" s="67"/>
       <c r="AG76" s="37"/>
-      <c r="AL76" s="79">
-        <f>SUM(AL68:AN73)</f>
-        <v>1000000</v>
-      </c>
+      <c r="AL76" s="79"/>
       <c r="AM76" s="79"/>
       <c r="AN76" s="59"/>
       <c r="AV76" s="6"/>
@@ -5696,80 +5689,80 @@
     <row r="77" spans="1:48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="94"/>
       <c r="B77" s="5"/>
-      <c r="C77" s="205" t="s">
+      <c r="C77" s="202" t="s">
         <v>64</v>
       </c>
-      <c r="D77" s="206"/>
-      <c r="E77" s="206"/>
-      <c r="F77" s="206"/>
-      <c r="G77" s="206"/>
-      <c r="H77" s="206"/>
-      <c r="I77" s="206"/>
-      <c r="J77" s="206"/>
-      <c r="K77" s="206"/>
-      <c r="L77" s="206"/>
-      <c r="M77" s="206"/>
-      <c r="N77" s="206"/>
-      <c r="O77" s="206"/>
-      <c r="P77" s="206"/>
-      <c r="Q77" s="206"/>
-      <c r="R77" s="206"/>
-      <c r="S77" s="206"/>
-      <c r="T77" s="206"/>
-      <c r="U77" s="206"/>
-      <c r="V77" s="206"/>
-      <c r="W77" s="206"/>
-      <c r="X77" s="206"/>
-      <c r="Y77" s="206"/>
-      <c r="Z77" s="206"/>
-      <c r="AA77" s="206"/>
-      <c r="AB77" s="206"/>
-      <c r="AC77" s="207"/>
+      <c r="D77" s="203"/>
+      <c r="E77" s="203"/>
+      <c r="F77" s="203"/>
+      <c r="G77" s="203"/>
+      <c r="H77" s="203"/>
+      <c r="I77" s="203"/>
+      <c r="J77" s="203"/>
+      <c r="K77" s="203"/>
+      <c r="L77" s="203"/>
+      <c r="M77" s="203"/>
+      <c r="N77" s="203"/>
+      <c r="O77" s="203"/>
+      <c r="P77" s="203"/>
+      <c r="Q77" s="203"/>
+      <c r="R77" s="203"/>
+      <c r="S77" s="203"/>
+      <c r="T77" s="203"/>
+      <c r="U77" s="203"/>
+      <c r="V77" s="203"/>
+      <c r="W77" s="203"/>
+      <c r="X77" s="203"/>
+      <c r="Y77" s="203"/>
+      <c r="Z77" s="203"/>
+      <c r="AA77" s="203"/>
+      <c r="AB77" s="203"/>
+      <c r="AC77" s="204"/>
       <c r="AG77" s="37"/>
-      <c r="AH77" s="137" t="s">
+      <c r="AH77" s="134" t="s">
         <v>56</v>
       </c>
-      <c r="AI77" s="137"/>
-      <c r="AJ77" s="137"/>
-      <c r="AK77" s="137"/>
-      <c r="AL77" s="183">
+      <c r="AI77" s="134"/>
+      <c r="AJ77" s="134"/>
+      <c r="AK77" s="134"/>
+      <c r="AL77" s="180">
         <f>SUM(AL69:AN73)</f>
         <v>1000000</v>
       </c>
-      <c r="AM77" s="183"/>
-      <c r="AN77" s="184"/>
+      <c r="AM77" s="180"/>
+      <c r="AN77" s="181"/>
       <c r="AV77" s="6"/>
     </row>
     <row r="78" spans="1:48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="94"/>
       <c r="B78" s="5"/>
-      <c r="C78" s="205"/>
-      <c r="D78" s="206"/>
-      <c r="E78" s="206"/>
-      <c r="F78" s="206"/>
-      <c r="G78" s="206"/>
-      <c r="H78" s="206"/>
-      <c r="I78" s="206"/>
-      <c r="J78" s="206"/>
-      <c r="K78" s="206"/>
-      <c r="L78" s="206"/>
-      <c r="M78" s="206"/>
-      <c r="N78" s="206"/>
-      <c r="O78" s="206"/>
-      <c r="P78" s="206"/>
-      <c r="Q78" s="206"/>
-      <c r="R78" s="206"/>
-      <c r="S78" s="206"/>
-      <c r="T78" s="206"/>
-      <c r="U78" s="206"/>
-      <c r="V78" s="206"/>
-      <c r="W78" s="206"/>
-      <c r="X78" s="206"/>
-      <c r="Y78" s="206"/>
-      <c r="Z78" s="206"/>
-      <c r="AA78" s="206"/>
-      <c r="AB78" s="206"/>
-      <c r="AC78" s="207"/>
+      <c r="C78" s="202"/>
+      <c r="D78" s="203"/>
+      <c r="E78" s="203"/>
+      <c r="F78" s="203"/>
+      <c r="G78" s="203"/>
+      <c r="H78" s="203"/>
+      <c r="I78" s="203"/>
+      <c r="J78" s="203"/>
+      <c r="K78" s="203"/>
+      <c r="L78" s="203"/>
+      <c r="M78" s="203"/>
+      <c r="N78" s="203"/>
+      <c r="O78" s="203"/>
+      <c r="P78" s="203"/>
+      <c r="Q78" s="203"/>
+      <c r="R78" s="203"/>
+      <c r="S78" s="203"/>
+      <c r="T78" s="203"/>
+      <c r="U78" s="203"/>
+      <c r="V78" s="203"/>
+      <c r="W78" s="203"/>
+      <c r="X78" s="203"/>
+      <c r="Y78" s="203"/>
+      <c r="Z78" s="203"/>
+      <c r="AA78" s="203"/>
+      <c r="AB78" s="203"/>
+      <c r="AC78" s="204"/>
       <c r="AG78" s="37"/>
       <c r="AL78" s="79"/>
       <c r="AM78" s="109"/>
@@ -5779,77 +5772,77 @@
     <row r="79" spans="1:48" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="94"/>
       <c r="B79" s="5"/>
-      <c r="C79" s="205"/>
-      <c r="D79" s="206"/>
-      <c r="E79" s="206"/>
-      <c r="F79" s="206"/>
-      <c r="G79" s="206"/>
-      <c r="H79" s="206"/>
-      <c r="I79" s="206"/>
-      <c r="J79" s="206"/>
-      <c r="K79" s="206"/>
-      <c r="L79" s="206"/>
-      <c r="M79" s="206"/>
-      <c r="N79" s="206"/>
-      <c r="O79" s="206"/>
-      <c r="P79" s="206"/>
-      <c r="Q79" s="206"/>
-      <c r="R79" s="206"/>
-      <c r="S79" s="206"/>
-      <c r="T79" s="206"/>
-      <c r="U79" s="206"/>
-      <c r="V79" s="206"/>
-      <c r="W79" s="206"/>
-      <c r="X79" s="206"/>
-      <c r="Y79" s="206"/>
-      <c r="Z79" s="206"/>
-      <c r="AA79" s="206"/>
-      <c r="AB79" s="206"/>
-      <c r="AC79" s="207"/>
+      <c r="C79" s="202"/>
+      <c r="D79" s="203"/>
+      <c r="E79" s="203"/>
+      <c r="F79" s="203"/>
+      <c r="G79" s="203"/>
+      <c r="H79" s="203"/>
+      <c r="I79" s="203"/>
+      <c r="J79" s="203"/>
+      <c r="K79" s="203"/>
+      <c r="L79" s="203"/>
+      <c r="M79" s="203"/>
+      <c r="N79" s="203"/>
+      <c r="O79" s="203"/>
+      <c r="P79" s="203"/>
+      <c r="Q79" s="203"/>
+      <c r="R79" s="203"/>
+      <c r="S79" s="203"/>
+      <c r="T79" s="203"/>
+      <c r="U79" s="203"/>
+      <c r="V79" s="203"/>
+      <c r="W79" s="203"/>
+      <c r="X79" s="203"/>
+      <c r="Y79" s="203"/>
+      <c r="Z79" s="203"/>
+      <c r="AA79" s="203"/>
+      <c r="AB79" s="203"/>
+      <c r="AC79" s="204"/>
       <c r="AG79" s="37"/>
-      <c r="AH79" s="137" t="s">
+      <c r="AH79" s="134" t="s">
         <v>65</v>
       </c>
-      <c r="AI79" s="138"/>
-      <c r="AJ79" s="138"/>
-      <c r="AK79" s="138"/>
-      <c r="AL79" s="203">
+      <c r="AI79" s="135"/>
+      <c r="AJ79" s="135"/>
+      <c r="AK79" s="135"/>
+      <c r="AL79" s="200">
         <v>0.8</v>
       </c>
-      <c r="AM79" s="203"/>
-      <c r="AN79" s="204"/>
+      <c r="AM79" s="200"/>
+      <c r="AN79" s="201"/>
       <c r="AV79" s="6"/>
     </row>
     <row r="80" spans="1:48" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="94"/>
       <c r="B80" s="5"/>
-      <c r="C80" s="205"/>
-      <c r="D80" s="206"/>
-      <c r="E80" s="206"/>
-      <c r="F80" s="206"/>
-      <c r="G80" s="206"/>
-      <c r="H80" s="206"/>
-      <c r="I80" s="206"/>
-      <c r="J80" s="206"/>
-      <c r="K80" s="206"/>
-      <c r="L80" s="206"/>
-      <c r="M80" s="206"/>
-      <c r="N80" s="206"/>
-      <c r="O80" s="206"/>
-      <c r="P80" s="206"/>
-      <c r="Q80" s="206"/>
-      <c r="R80" s="206"/>
-      <c r="S80" s="206"/>
-      <c r="T80" s="206"/>
-      <c r="U80" s="206"/>
-      <c r="V80" s="206"/>
-      <c r="W80" s="206"/>
-      <c r="X80" s="206"/>
-      <c r="Y80" s="206"/>
-      <c r="Z80" s="206"/>
-      <c r="AA80" s="206"/>
-      <c r="AB80" s="206"/>
-      <c r="AC80" s="207"/>
+      <c r="C80" s="202"/>
+      <c r="D80" s="203"/>
+      <c r="E80" s="203"/>
+      <c r="F80" s="203"/>
+      <c r="G80" s="203"/>
+      <c r="H80" s="203"/>
+      <c r="I80" s="203"/>
+      <c r="J80" s="203"/>
+      <c r="K80" s="203"/>
+      <c r="L80" s="203"/>
+      <c r="M80" s="203"/>
+      <c r="N80" s="203"/>
+      <c r="O80" s="203"/>
+      <c r="P80" s="203"/>
+      <c r="Q80" s="203"/>
+      <c r="R80" s="203"/>
+      <c r="S80" s="203"/>
+      <c r="T80" s="203"/>
+      <c r="U80" s="203"/>
+      <c r="V80" s="203"/>
+      <c r="W80" s="203"/>
+      <c r="X80" s="203"/>
+      <c r="Y80" s="203"/>
+      <c r="Z80" s="203"/>
+      <c r="AA80" s="203"/>
+      <c r="AB80" s="203"/>
+      <c r="AC80" s="204"/>
       <c r="AG80" s="37"/>
       <c r="AL80" s="79"/>
       <c r="AM80" s="79"/>
@@ -5859,87 +5852,87 @@
     <row r="81" spans="1:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="94"/>
       <c r="B81" s="5"/>
-      <c r="C81" s="205"/>
-      <c r="D81" s="206"/>
-      <c r="E81" s="206"/>
-      <c r="F81" s="206"/>
-      <c r="G81" s="206"/>
-      <c r="H81" s="206"/>
-      <c r="I81" s="206"/>
-      <c r="J81" s="206"/>
-      <c r="K81" s="206"/>
-      <c r="L81" s="206"/>
-      <c r="M81" s="206"/>
-      <c r="N81" s="206"/>
-      <c r="O81" s="206"/>
-      <c r="P81" s="206"/>
-      <c r="Q81" s="206"/>
-      <c r="R81" s="206"/>
-      <c r="S81" s="206"/>
-      <c r="T81" s="206"/>
-      <c r="U81" s="206"/>
-      <c r="V81" s="206"/>
-      <c r="W81" s="206"/>
-      <c r="X81" s="206"/>
-      <c r="Y81" s="206"/>
-      <c r="Z81" s="206"/>
-      <c r="AA81" s="206"/>
-      <c r="AB81" s="206"/>
-      <c r="AC81" s="207"/>
+      <c r="C81" s="202"/>
+      <c r="D81" s="203"/>
+      <c r="E81" s="203"/>
+      <c r="F81" s="203"/>
+      <c r="G81" s="203"/>
+      <c r="H81" s="203"/>
+      <c r="I81" s="203"/>
+      <c r="J81" s="203"/>
+      <c r="K81" s="203"/>
+      <c r="L81" s="203"/>
+      <c r="M81" s="203"/>
+      <c r="N81" s="203"/>
+      <c r="O81" s="203"/>
+      <c r="P81" s="203"/>
+      <c r="Q81" s="203"/>
+      <c r="R81" s="203"/>
+      <c r="S81" s="203"/>
+      <c r="T81" s="203"/>
+      <c r="U81" s="203"/>
+      <c r="V81" s="203"/>
+      <c r="W81" s="203"/>
+      <c r="X81" s="203"/>
+      <c r="Y81" s="203"/>
+      <c r="Z81" s="203"/>
+      <c r="AA81" s="203"/>
+      <c r="AB81" s="203"/>
+      <c r="AC81" s="204"/>
       <c r="AG81" s="37"/>
-      <c r="AH81" s="137" t="s">
+      <c r="AH81" s="134" t="s">
         <v>66</v>
       </c>
-      <c r="AI81" s="138"/>
-      <c r="AJ81" s="138"/>
-      <c r="AK81" s="138"/>
-      <c r="AL81" s="211">
+      <c r="AI81" s="135"/>
+      <c r="AJ81" s="135"/>
+      <c r="AK81" s="135"/>
+      <c r="AL81" s="208">
         <f>ROUND(SUM(AL79*AL77),0)</f>
         <v>800000</v>
       </c>
-      <c r="AM81" s="211"/>
-      <c r="AN81" s="212"/>
-      <c r="AQ81" s="145"/>
-      <c r="AR81" s="145"/>
-      <c r="AS81" s="145"/>
-      <c r="AT81" s="145"/>
-      <c r="AU81" s="145"/>
-      <c r="AV81" s="145"/>
-      <c r="AW81" s="145"/>
-      <c r="AX81" s="145"/>
-      <c r="AY81" s="145"/>
-      <c r="AZ81" s="145"/>
+      <c r="AM81" s="208"/>
+      <c r="AN81" s="209"/>
+      <c r="AQ81" s="142"/>
+      <c r="AR81" s="142"/>
+      <c r="AS81" s="142"/>
+      <c r="AT81" s="142"/>
+      <c r="AU81" s="142"/>
+      <c r="AV81" s="142"/>
+      <c r="AW81" s="142"/>
+      <c r="AX81" s="142"/>
+      <c r="AY81" s="142"/>
+      <c r="AZ81" s="142"/>
     </row>
     <row r="82" spans="1:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="94"/>
       <c r="B82" s="5"/>
-      <c r="C82" s="208"/>
-      <c r="D82" s="209"/>
-      <c r="E82" s="209"/>
-      <c r="F82" s="209"/>
-      <c r="G82" s="209"/>
-      <c r="H82" s="209"/>
-      <c r="I82" s="209"/>
-      <c r="J82" s="209"/>
-      <c r="K82" s="209"/>
-      <c r="L82" s="209"/>
-      <c r="M82" s="209"/>
-      <c r="N82" s="209"/>
-      <c r="O82" s="209"/>
-      <c r="P82" s="209"/>
-      <c r="Q82" s="209"/>
-      <c r="R82" s="209"/>
-      <c r="S82" s="209"/>
-      <c r="T82" s="209"/>
-      <c r="U82" s="209"/>
-      <c r="V82" s="209"/>
-      <c r="W82" s="209"/>
-      <c r="X82" s="209"/>
-      <c r="Y82" s="209"/>
-      <c r="Z82" s="209"/>
-      <c r="AA82" s="209"/>
-      <c r="AB82" s="209"/>
-      <c r="AC82" s="210"/>
+      <c r="C82" s="205"/>
+      <c r="D82" s="206"/>
+      <c r="E82" s="206"/>
+      <c r="F82" s="206"/>
+      <c r="G82" s="206"/>
+      <c r="H82" s="206"/>
+      <c r="I82" s="206"/>
+      <c r="J82" s="206"/>
+      <c r="K82" s="206"/>
+      <c r="L82" s="206"/>
+      <c r="M82" s="206"/>
+      <c r="N82" s="206"/>
+      <c r="O82" s="206"/>
+      <c r="P82" s="206"/>
+      <c r="Q82" s="206"/>
+      <c r="R82" s="206"/>
+      <c r="S82" s="206"/>
+      <c r="T82" s="206"/>
+      <c r="U82" s="206"/>
+      <c r="V82" s="206"/>
+      <c r="W82" s="206"/>
+      <c r="X82" s="206"/>
+      <c r="Y82" s="206"/>
+      <c r="Z82" s="206"/>
+      <c r="AA82" s="206"/>
+      <c r="AB82" s="206"/>
+      <c r="AC82" s="207"/>
       <c r="AG82" s="37"/>
       <c r="AN82" s="18"/>
       <c r="AV82" s="6"/>
@@ -6019,33 +6012,33 @@
       <c r="L86" s="122"/>
       <c r="M86" s="122"/>
       <c r="N86" s="122"/>
-      <c r="O86" s="132" t="s">
+      <c r="O86" s="129" t="s">
         <v>68</v>
       </c>
-      <c r="P86" s="133"/>
-      <c r="Q86" s="133"/>
-      <c r="R86" s="133"/>
-      <c r="S86" s="133"/>
-      <c r="T86" s="133"/>
-      <c r="U86" s="133"/>
-      <c r="V86" s="133"/>
-      <c r="W86" s="133"/>
-      <c r="X86" s="133"/>
-      <c r="Y86" s="133"/>
-      <c r="Z86" s="133"/>
-      <c r="AA86" s="133"/>
-      <c r="AB86" s="133"/>
-      <c r="AC86" s="133"/>
-      <c r="AD86" s="133"/>
-      <c r="AE86" s="133"/>
-      <c r="AF86" s="133"/>
-      <c r="AG86" s="133"/>
-      <c r="AH86" s="133"/>
-      <c r="AI86" s="133"/>
-      <c r="AJ86" s="133"/>
-      <c r="AK86" s="133"/>
-      <c r="AL86" s="133"/>
-      <c r="AM86" s="133"/>
+      <c r="P86" s="130"/>
+      <c r="Q86" s="130"/>
+      <c r="R86" s="130"/>
+      <c r="S86" s="130"/>
+      <c r="T86" s="130"/>
+      <c r="U86" s="130"/>
+      <c r="V86" s="130"/>
+      <c r="W86" s="130"/>
+      <c r="X86" s="130"/>
+      <c r="Y86" s="130"/>
+      <c r="Z86" s="130"/>
+      <c r="AA86" s="130"/>
+      <c r="AB86" s="130"/>
+      <c r="AC86" s="130"/>
+      <c r="AD86" s="130"/>
+      <c r="AE86" s="130"/>
+      <c r="AF86" s="130"/>
+      <c r="AG86" s="130"/>
+      <c r="AH86" s="130"/>
+      <c r="AI86" s="130"/>
+      <c r="AJ86" s="130"/>
+      <c r="AK86" s="130"/>
+      <c r="AL86" s="130"/>
+      <c r="AM86" s="130"/>
       <c r="AN86" s="18"/>
       <c r="AV86" s="6"/>
     </row>
@@ -6066,31 +6059,31 @@
       <c r="L87" s="128"/>
       <c r="M87" s="128"/>
       <c r="N87" s="128"/>
-      <c r="O87" s="133"/>
-      <c r="P87" s="133"/>
-      <c r="Q87" s="133"/>
-      <c r="R87" s="133"/>
-      <c r="S87" s="133"/>
-      <c r="T87" s="133"/>
-      <c r="U87" s="133"/>
-      <c r="V87" s="133"/>
-      <c r="W87" s="133"/>
-      <c r="X87" s="133"/>
-      <c r="Y87" s="133"/>
-      <c r="Z87" s="133"/>
-      <c r="AA87" s="133"/>
-      <c r="AB87" s="133"/>
-      <c r="AC87" s="133"/>
-      <c r="AD87" s="133"/>
-      <c r="AE87" s="133"/>
-      <c r="AF87" s="133"/>
-      <c r="AG87" s="133"/>
-      <c r="AH87" s="133"/>
-      <c r="AI87" s="133"/>
-      <c r="AJ87" s="133"/>
-      <c r="AK87" s="133"/>
-      <c r="AL87" s="133"/>
-      <c r="AM87" s="133"/>
+      <c r="O87" s="130"/>
+      <c r="P87" s="130"/>
+      <c r="Q87" s="130"/>
+      <c r="R87" s="130"/>
+      <c r="S87" s="130"/>
+      <c r="T87" s="130"/>
+      <c r="U87" s="130"/>
+      <c r="V87" s="130"/>
+      <c r="W87" s="130"/>
+      <c r="X87" s="130"/>
+      <c r="Y87" s="130"/>
+      <c r="Z87" s="130"/>
+      <c r="AA87" s="130"/>
+      <c r="AB87" s="130"/>
+      <c r="AC87" s="130"/>
+      <c r="AD87" s="130"/>
+      <c r="AE87" s="130"/>
+      <c r="AF87" s="130"/>
+      <c r="AG87" s="130"/>
+      <c r="AH87" s="130"/>
+      <c r="AI87" s="130"/>
+      <c r="AJ87" s="130"/>
+      <c r="AK87" s="130"/>
+      <c r="AL87" s="130"/>
+      <c r="AM87" s="130"/>
       <c r="AN87" s="18"/>
       <c r="AT87" s="39"/>
       <c r="AV87" s="6"/>
@@ -6098,43 +6091,43 @@
     <row r="88" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="94"/>
       <c r="B88" s="5"/>
-      <c r="C88" s="129"/>
-      <c r="D88" s="129"/>
-      <c r="E88" s="129"/>
-      <c r="F88" s="129"/>
-      <c r="G88" s="129"/>
-      <c r="H88" s="129"/>
-      <c r="I88" s="129"/>
-      <c r="J88" s="129"/>
-      <c r="K88" s="129"/>
-      <c r="L88" s="129"/>
-      <c r="M88" s="129"/>
-      <c r="N88" s="129"/>
-      <c r="O88" s="133"/>
-      <c r="P88" s="133"/>
-      <c r="Q88" s="133"/>
-      <c r="R88" s="133"/>
-      <c r="S88" s="133"/>
-      <c r="T88" s="133"/>
-      <c r="U88" s="133"/>
-      <c r="V88" s="133"/>
-      <c r="W88" s="133"/>
-      <c r="X88" s="133"/>
-      <c r="Y88" s="133"/>
-      <c r="Z88" s="133"/>
-      <c r="AA88" s="133"/>
-      <c r="AB88" s="133"/>
-      <c r="AC88" s="133"/>
-      <c r="AD88" s="133"/>
-      <c r="AE88" s="133"/>
-      <c r="AF88" s="133"/>
-      <c r="AG88" s="133"/>
-      <c r="AH88" s="133"/>
-      <c r="AI88" s="133"/>
-      <c r="AJ88" s="133"/>
-      <c r="AK88" s="133"/>
-      <c r="AL88" s="133"/>
-      <c r="AM88" s="133"/>
+      <c r="C88" s="257"/>
+      <c r="D88" s="257"/>
+      <c r="E88" s="257"/>
+      <c r="F88" s="257"/>
+      <c r="G88" s="257"/>
+      <c r="H88" s="257"/>
+      <c r="I88" s="257"/>
+      <c r="J88" s="257"/>
+      <c r="K88" s="257"/>
+      <c r="L88" s="257"/>
+      <c r="M88" s="257"/>
+      <c r="N88" s="257"/>
+      <c r="O88" s="130"/>
+      <c r="P88" s="130"/>
+      <c r="Q88" s="130"/>
+      <c r="R88" s="130"/>
+      <c r="S88" s="130"/>
+      <c r="T88" s="130"/>
+      <c r="U88" s="130"/>
+      <c r="V88" s="130"/>
+      <c r="W88" s="130"/>
+      <c r="X88" s="130"/>
+      <c r="Y88" s="130"/>
+      <c r="Z88" s="130"/>
+      <c r="AA88" s="130"/>
+      <c r="AB88" s="130"/>
+      <c r="AC88" s="130"/>
+      <c r="AD88" s="130"/>
+      <c r="AE88" s="130"/>
+      <c r="AF88" s="130"/>
+      <c r="AG88" s="130"/>
+      <c r="AH88" s="130"/>
+      <c r="AI88" s="130"/>
+      <c r="AJ88" s="130"/>
+      <c r="AK88" s="130"/>
+      <c r="AL88" s="130"/>
+      <c r="AM88" s="130"/>
       <c r="AN88" s="18"/>
       <c r="AT88" s="39"/>
       <c r="AV88" s="6"/>
@@ -6142,28 +6135,28 @@
     <row r="89" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="94"/>
       <c r="B89" s="5"/>
-      <c r="C89" s="130"/>
-      <c r="D89" s="130"/>
-      <c r="E89" s="130"/>
-      <c r="F89" s="130"/>
-      <c r="G89" s="130"/>
-      <c r="H89" s="130"/>
-      <c r="I89" s="130"/>
-      <c r="J89" s="130"/>
-      <c r="K89" s="130"/>
-      <c r="L89" s="130"/>
-      <c r="M89" s="130"/>
-      <c r="N89" s="130"/>
-      <c r="P89" s="136"/>
-      <c r="Q89" s="136"/>
-      <c r="R89" s="136"/>
-      <c r="S89" s="136"/>
-      <c r="T89" s="136"/>
-      <c r="U89" s="136"/>
-      <c r="V89" s="136"/>
-      <c r="W89" s="136"/>
-      <c r="X89" s="136"/>
-      <c r="Y89" s="136"/>
+      <c r="C89" s="68"/>
+      <c r="D89" s="68"/>
+      <c r="E89" s="68"/>
+      <c r="F89" s="68"/>
+      <c r="G89" s="68"/>
+      <c r="H89" s="68"/>
+      <c r="I89" s="68"/>
+      <c r="J89" s="68"/>
+      <c r="K89" s="68"/>
+      <c r="L89" s="68"/>
+      <c r="M89" s="68"/>
+      <c r="N89" s="68"/>
+      <c r="P89" s="133"/>
+      <c r="Q89" s="133"/>
+      <c r="R89" s="133"/>
+      <c r="S89" s="133"/>
+      <c r="T89" s="133"/>
+      <c r="U89" s="133"/>
+      <c r="V89" s="133"/>
+      <c r="W89" s="133"/>
+      <c r="X89" s="133"/>
+      <c r="Y89" s="133"/>
       <c r="AA89" s="68"/>
       <c r="AB89" s="68"/>
       <c r="AC89" s="68"/>
@@ -6186,18 +6179,18 @@
         <v>70</v>
       </c>
       <c r="B90" s="5"/>
-      <c r="C90" s="131"/>
-      <c r="D90" s="131"/>
-      <c r="E90" s="131"/>
-      <c r="F90" s="131"/>
-      <c r="G90" s="131"/>
-      <c r="H90" s="131"/>
-      <c r="I90" s="131"/>
-      <c r="J90" s="131"/>
-      <c r="K90" s="131"/>
-      <c r="L90" s="131"/>
-      <c r="M90" s="131"/>
-      <c r="N90" s="131"/>
+      <c r="C90" s="258"/>
+      <c r="D90" s="258"/>
+      <c r="E90" s="258"/>
+      <c r="F90" s="258"/>
+      <c r="G90" s="258"/>
+      <c r="H90" s="258"/>
+      <c r="I90" s="258"/>
+      <c r="J90" s="258"/>
+      <c r="K90" s="258"/>
+      <c r="L90" s="258"/>
+      <c r="M90" s="258"/>
+      <c r="N90" s="258"/>
       <c r="P90" s="122"/>
       <c r="Q90" s="122"/>
       <c r="R90" s="122"/>
@@ -6228,20 +6221,20 @@
     <row r="91" spans="1:52" ht="14.5" x14ac:dyDescent="0.3">
       <c r="A91" s="94"/>
       <c r="B91" s="5"/>
-      <c r="C91" s="134" t="s">
+      <c r="C91" s="131" t="s">
         <v>71</v>
       </c>
-      <c r="D91" s="134"/>
-      <c r="E91" s="134"/>
-      <c r="F91" s="134"/>
-      <c r="G91" s="134"/>
-      <c r="H91" s="134"/>
-      <c r="I91" s="134"/>
-      <c r="J91" s="134"/>
-      <c r="K91" s="134"/>
-      <c r="L91" s="134"/>
-      <c r="M91" s="134"/>
-      <c r="N91" s="134"/>
+      <c r="D91" s="131"/>
+      <c r="E91" s="131"/>
+      <c r="F91" s="131"/>
+      <c r="G91" s="131"/>
+      <c r="H91" s="131"/>
+      <c r="I91" s="131"/>
+      <c r="J91" s="131"/>
+      <c r="K91" s="131"/>
+      <c r="L91" s="131"/>
+      <c r="M91" s="131"/>
+      <c r="N91" s="131"/>
       <c r="O91" s="44"/>
       <c r="P91" s="108" t="s">
         <v>72</v>
@@ -6256,19 +6249,19 @@
       <c r="X91" s="108"/>
       <c r="Y91" s="108"/>
       <c r="Z91" s="44"/>
-      <c r="AC91" s="135" t="s">
+      <c r="AC91" s="132" t="s">
         <v>73</v>
       </c>
-      <c r="AD91" s="135"/>
-      <c r="AE91" s="135"/>
-      <c r="AF91" s="135"/>
-      <c r="AG91" s="135"/>
-      <c r="AH91" s="135"/>
-      <c r="AI91" s="135"/>
-      <c r="AJ91" s="135"/>
-      <c r="AK91" s="135"/>
-      <c r="AL91" s="135"/>
-      <c r="AM91" s="135"/>
+      <c r="AD91" s="132"/>
+      <c r="AE91" s="132"/>
+      <c r="AF91" s="132"/>
+      <c r="AG91" s="132"/>
+      <c r="AH91" s="132"/>
+      <c r="AI91" s="132"/>
+      <c r="AJ91" s="132"/>
+      <c r="AK91" s="132"/>
+      <c r="AL91" s="132"/>
+      <c r="AM91" s="132"/>
       <c r="AN91" s="18"/>
       <c r="AT91" s="39"/>
       <c r="AV91" s="6"/>
@@ -7097,7 +7090,7 @@
   <protectedRanges>
     <protectedRange sqref="W14" name="Purchase Order" securityDescriptor="O:WDG:WDD:(A;;CC;;;S-1-5-21-2063348182-967534376-2122337923-1195)(A;;CC;;;S-1-5-21-2063348182-967534376-2122337923-1201)(A;;CC;;;S-1-5-21-2063348182-967534376-2122337923-2061)(A;;CC;;;S-1-5-21-2063348182-967534376-2122337923-1751)"/>
   </protectedRanges>
-  <mergeCells count="122">
+  <mergeCells count="121">
     <mergeCell ref="AQ6:AS6"/>
     <mergeCell ref="AG13:AM13"/>
     <mergeCell ref="C7:U9"/>
@@ -7208,7 +7201,6 @@
     <mergeCell ref="W39:AC39"/>
     <mergeCell ref="C87:N88"/>
     <mergeCell ref="C86:N86"/>
-    <mergeCell ref="C89:N90"/>
     <mergeCell ref="O86:AM88"/>
     <mergeCell ref="C91:N91"/>
     <mergeCell ref="AC91:AM91"/>
@@ -7252,42 +7244,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="25.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="255" t="s">
+      <c r="A1" s="252" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="256"/>
+      <c r="B1" s="253"/>
     </row>
     <row r="2" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="88"/>
       <c r="B2" s="88"/>
     </row>
     <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="257" t="s">
+      <c r="A3" s="254" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="257"/>
+      <c r="B3" s="254"/>
     </row>
     <row r="4" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="257" t="s">
+      <c r="A4" s="254" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="257"/>
+      <c r="B4" s="254"/>
     </row>
     <row r="5" spans="1:2" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="107"/>
       <c r="B5" s="107"/>
     </row>
     <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.3">
-      <c r="A6" s="258" t="s">
+      <c r="A6" s="255" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="258"/>
+      <c r="B6" s="255"/>
     </row>
     <row r="7" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="259" t="s">
+      <c r="A7" s="256" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="259"/>
+      <c r="B7" s="256"/>
     </row>
     <row r="8" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="88"/>
@@ -7431,10 +7423,10 @@
       <c r="B27" s="90"/>
     </row>
     <row r="28" spans="1:2" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="253" t="s">
+      <c r="A28" s="250" t="s">
         <v>112</v>
       </c>
-      <c r="B28" s="254"/>
+      <c r="B28" s="251"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -7454,6 +7446,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FBEA0C5774296845BFB6FE77C932CCE7" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="970475546e7465e72c9a0b3d97abf172">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65e72d04-2228-4267-b051-35e609b4345c" xmlns:ns3="1d0e33f6-ce45-4db7-97d8-68b11b29cade" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a808934f6ec18dd59b9090d4b95201c0" ns2:_="" ns3:_="">
     <xsd:import namespace="65e72d04-2228-4267-b051-35e609b4345c"/>
@@ -7670,7 +7666,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="1d0e33f6-ce45-4db7-97d8-68b11b29cade">
@@ -7699,7 +7695,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -7708,11 +7704,15 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5F59B31-FAD6-42A0-86F6-B588DC513FFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC9F0358-5361-444B-864C-5365A4B5D8C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7731,7 +7731,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCDA9C15-FC5A-47AA-8973-D36B53905EE6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -7748,18 +7748,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{744CCE99-E6B0-4BFC-992F-ECFE64466B9F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5F59B31-FAD6-42A0-86F6-B588DC513FFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>